<commit_message>
week 5 - updated exam results
</commit_message>
<xml_diff>
--- a/exam_results/Participants_2.xlsx
+++ b/exam_results/Participants_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Desktop/2024_anlp/anlp2024_fall/exam_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17866FC-863C-5B42-B629-64CA92F90922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DF5929-43FF-DB41-B693-83C76B83C240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34560" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="355">
   <si>
     <t>Ad</t>
   </si>
@@ -1085,12 +1085,6 @@
   </si>
   <si>
     <t>Hmw2</t>
-  </si>
-  <si>
-    <t>*****</t>
-  </si>
-  <si>
-    <t>****</t>
   </si>
 </sst>
 </file>
@@ -1448,8 +1442,8 @@
   <dimension ref="A1:E118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" activeCellId="1" sqref="C64 C63"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1667,7 +1661,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1681,7 +1675,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1695,7 +1689,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1709,7 +1703,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -1723,7 +1717,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -1734,7 +1728,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1745,7 +1739,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>66</v>
       </c>
@@ -1756,7 +1750,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -1767,7 +1761,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -1777,11 +1771,11 @@
       <c r="C25" t="s">
         <v>74</v>
       </c>
-      <c r="E25" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -1795,7 +1789,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>78</v>
       </c>
@@ -1809,7 +1803,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -1823,7 +1817,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -1834,7 +1828,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -1845,7 +1839,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>89</v>
       </c>
@@ -1859,7 +1853,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -2488,7 +2482,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>239</v>
       </c>
@@ -2502,7 +2496,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>242</v>
       </c>
@@ -2516,7 +2510,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>245</v>
       </c>
@@ -2530,7 +2524,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>248</v>
       </c>
@@ -2541,7 +2535,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>251</v>
       </c>
@@ -2555,7 +2549,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>254</v>
       </c>
@@ -2565,11 +2559,11 @@
       <c r="C86" t="s">
         <v>256</v>
       </c>
-      <c r="E86" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D86">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>257</v>
       </c>
@@ -2580,7 +2574,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>260</v>
       </c>
@@ -2591,7 +2585,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>263</v>
       </c>
@@ -2602,7 +2596,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>266</v>
       </c>
@@ -2616,7 +2610,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>269</v>
       </c>
@@ -2627,7 +2621,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>272</v>
       </c>
@@ -2638,7 +2632,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>275</v>
       </c>
@@ -2652,7 +2646,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>278</v>
       </c>
@@ -2666,7 +2660,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>281</v>
       </c>
@@ -2680,7 +2674,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>284</v>
       </c>

</xml_diff>

<commit_message>
midterm results - ka
</commit_message>
<xml_diff>
--- a/exam_results/Participants_2.xlsx
+++ b/exam_results/Participants_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Desktop/2024_anlp/anlp2024_fall/exam_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E295F5-45E0-6249-9748-875952E8881F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE036A0-EC31-BB46-A81C-1C3DE969FA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1461,8 +1461,8 @@
   <dimension ref="A1:H118"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2510,7 +2510,7 @@
         <v>217</v>
       </c>
       <c r="D73">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="E73">
         <v>70</v>

</xml_diff>

<commit_message>
homework 2 results updates
</commit_message>
<xml_diff>
--- a/exam_results/Participants_2.xlsx
+++ b/exam_results/Participants_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Desktop/2024_anlp/anlp2024_fall/exam_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA8BC03-8F82-184B-8A27-88568A2C5B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A251342-0F14-B94F-B4AB-E2BD147BB20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1476,9 +1476,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F76" sqref="F76"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2908,9 +2908,12 @@
       <c r="E66">
         <v>85</v>
       </c>
+      <c r="F66">
+        <v>100</v>
+      </c>
       <c r="I66">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
homework 2 results updates 2
</commit_message>
<xml_diff>
--- a/exam_results/Participants_2.xlsx
+++ b/exam_results/Participants_2.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Desktop/2024_anlp/anlp2024_fall/exam_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947AD5AC-5667-FB48-AA60-D317CB0C9FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C6BA8F-7027-4E42-B3ED-4B09E136277C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14140" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentManualCount="12"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1479,9 +1479,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G107" sqref="G107"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1613,6 +1613,9 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
+      <c r="D5">
+        <v>65</v>
+      </c>
       <c r="E5">
         <v>75</v>
       </c>
@@ -1621,11 +1624,11 @@
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>24.5</v>
+        <v>31</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>61.250000000000007</v>
+        <v>77.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1707,16 +1710,22 @@
       <c r="C9" t="s">
         <v>26</v>
       </c>
+      <c r="D9">
+        <v>55</v>
+      </c>
       <c r="E9">
         <v>85</v>
       </c>
+      <c r="F9">
+        <v>55</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="K9">
         <f t="shared" si="1"/>
-        <v>42.5</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1869,13 +1878,16 @@
       <c r="E15">
         <v>85</v>
       </c>
+      <c r="F15">
+        <v>55</v>
+      </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>31.5</v>
       </c>
       <c r="K15">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>78.75</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2347,6 +2359,9 @@
       <c r="C34" t="s">
         <v>100</v>
       </c>
+      <c r="D34">
+        <v>55</v>
+      </c>
       <c r="E34">
         <v>75</v>
       </c>
@@ -2355,11 +2370,11 @@
       </c>
       <c r="I34">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>28.5</v>
       </c>
       <c r="K34">
         <f t="shared" si="1"/>
-        <v>57.499999999999993</v>
+        <v>71.25</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -2740,16 +2755,22 @@
       <c r="C49" t="s">
         <v>145</v>
       </c>
+      <c r="D49">
+        <v>55</v>
+      </c>
       <c r="E49">
         <v>95</v>
       </c>
+      <c r="F49">
+        <v>55</v>
+      </c>
       <c r="I49">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="K49">
         <f t="shared" si="1"/>
-        <v>47.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2843,16 +2864,22 @@
       <c r="C53" t="s">
         <v>157</v>
       </c>
+      <c r="D53">
+        <v>55</v>
+      </c>
       <c r="E53">
         <v>65</v>
       </c>
+      <c r="F53">
+        <v>55</v>
+      </c>
       <c r="I53">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="K53">
         <f t="shared" si="1"/>
-        <v>32.5</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
@@ -2871,13 +2898,16 @@
       <c r="E54">
         <v>70</v>
       </c>
+      <c r="F54">
+        <v>60</v>
+      </c>
       <c r="I54">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="K54">
         <f t="shared" si="1"/>
-        <v>55.000000000000007</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -3024,13 +3054,16 @@
       <c r="E60">
         <v>65</v>
       </c>
+      <c r="F60">
+        <v>55</v>
+      </c>
       <c r="I60">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>28.5</v>
       </c>
       <c r="K60">
         <f t="shared" si="1"/>
-        <v>57.499999999999993</v>
+        <v>71.25</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -3118,6 +3151,9 @@
       <c r="C64" t="s">
         <v>190</v>
       </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
       <c r="E64">
         <v>80</v>
       </c>
@@ -3207,7 +3243,7 @@
         <v>33</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67:K127" si="3">(I67/40)*100</f>
+        <f t="shared" ref="K67:K118" si="3">(I67/40)*100</f>
         <v>82.5</v>
       </c>
     </row>
@@ -4036,16 +4072,22 @@
       <c r="C100" t="s">
         <v>298</v>
       </c>
+      <c r="D100">
+        <v>55</v>
+      </c>
       <c r="E100">
         <v>95</v>
       </c>
+      <c r="F100">
+        <v>55</v>
+      </c>
       <c r="I100">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="K100">
         <f t="shared" si="3"/>
-        <v>47.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
@@ -4064,13 +4106,16 @@
       <c r="E101">
         <v>85</v>
       </c>
+      <c r="F101">
+        <v>55</v>
+      </c>
       <c r="I101">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>25.5</v>
       </c>
       <c r="K101">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>63.749999999999993</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
homework 2 results updates 4
</commit_message>
<xml_diff>
--- a/exam_results/Participants_2.xlsx
+++ b/exam_results/Participants_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Desktop/2024_anlp/anlp2024_fall/exam_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC5D632-B460-5147-AE8C-39BDC54CD268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B59A98-5A9E-6743-87B2-93D55B67B676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4460" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1479,9 +1479,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F119" sqref="F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3100,16 +3100,22 @@
       <c r="C61" t="s">
         <v>181</v>
       </c>
+      <c r="D61">
+        <v>55</v>
+      </c>
       <c r="E61">
         <v>35</v>
       </c>
+      <c r="F61">
+        <v>55</v>
+      </c>
       <c r="I61">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="K61">
         <f t="shared" si="1"/>
-        <v>17.5</v>
+        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -3889,6 +3895,9 @@
       <c r="C91" t="s">
         <v>271</v>
       </c>
+      <c r="D91">
+        <v>55</v>
+      </c>
       <c r="E91">
         <v>55</v>
       </c>
@@ -3897,11 +3906,11 @@
       </c>
       <c r="I91">
         <f t="shared" si="2"/>
-        <v>19.5</v>
+        <v>25</v>
       </c>
       <c r="K91">
         <f t="shared" si="3"/>
-        <v>48.75</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
@@ -4069,6 +4078,9 @@
       </c>
       <c r="C98" t="s">
         <v>292</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
       </c>
       <c r="E98">
         <v>60</v>

</xml_diff>

<commit_message>
Final Scores for Midterms and Finals (Out of 100) - updated
</commit_message>
<xml_diff>
--- a/exam_results/Participants_2.xlsx
+++ b/exam_results/Participants_2.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Desktop/2024_anlp/anlp2024_fall/exam_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CA921D-1E8B-0B45-BA52-4C596D496A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF86BED-83BE-9044-BEEC-192F7E4A31B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$1:$H$117</definedName>
@@ -1169,18 +1170,12 @@
     <t>dikran 70 - furkan 40</t>
   </si>
   <si>
-    <t>Final + Proje (% 60)</t>
-  </si>
-  <si>
     <t>Vize Toplam Notunuzun %40</t>
   </si>
   <si>
     <t>Ders Başarı Notunuz</t>
   </si>
   <si>
-    <t>Final Toplam Notunuzun %60</t>
-  </si>
-  <si>
     <t>alttaki ikisi de 50 puan üstünden hesaplanır toplamı final sınavı yerine geçer</t>
   </si>
   <si>
@@ -1188,6 +1183,12 @@
   </si>
   <si>
     <t>Final : 50 üstünden</t>
+  </si>
+  <si>
+    <t>Final + Proje Toplam Notunuzun %60</t>
+  </si>
+  <si>
+    <t>Total Final</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1251,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1280,6 +1281,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1293,7 +1300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1332,6 +1339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2399,10 +2407,10 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I110" sqref="I110"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2416,25 +2424,25 @@
     <col min="7" max="7" width="11.5" style="9" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.83203125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="33.33203125" style="13" customWidth="1"/>
     <col min="11" max="11" width="23.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D1" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
       <c r="H1" s="16" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I1" s="16"/>
       <c r="J1" s="8" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2460,13 +2468,13 @@
         <v>351</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I2" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>382</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>376</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>350</v>
@@ -2603,16 +2611,16 @@
       <c r="H6">
         <v>45</v>
       </c>
-      <c r="I6">
-        <v>26</v>
+      <c r="I6" s="18">
+        <v>29</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="K6" s="4">
         <f t="shared" si="2"/>
-        <v>73.599999999999994</v>
+        <v>75.400000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2737,16 +2745,16 @@
       <c r="H10">
         <v>42.5</v>
       </c>
-      <c r="I10">
-        <v>23</v>
+      <c r="I10" s="18">
+        <v>28</v>
       </c>
       <c r="J10" s="13">
         <f t="shared" si="1"/>
-        <v>65.5</v>
+        <v>70.5</v>
       </c>
       <c r="K10" s="4">
         <f t="shared" si="2"/>
-        <v>67.3</v>
+        <v>70.3</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2813,16 +2821,16 @@
       <c r="H12">
         <v>40</v>
       </c>
-      <c r="I12">
-        <v>44</v>
+      <c r="I12" s="18">
+        <v>48</v>
       </c>
       <c r="J12" s="13">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="K12" s="4">
         <f t="shared" si="2"/>
-        <v>88.4</v>
+        <v>90.8</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2965,16 +2973,16 @@
       <c r="H16">
         <v>42.5</v>
       </c>
-      <c r="I16">
-        <v>28</v>
+      <c r="I16" s="18">
+        <v>30</v>
       </c>
       <c r="J16" s="13">
         <f t="shared" si="1"/>
-        <v>70.5</v>
+        <v>72.5</v>
       </c>
       <c r="K16" s="4">
         <f t="shared" si="2"/>
-        <v>73.8</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3000,19 +3008,19 @@
         <f t="shared" si="0"/>
         <v>81.25</v>
       </c>
-      <c r="H17">
-        <v>45</v>
+      <c r="H17" s="18">
+        <v>48</v>
       </c>
       <c r="I17">
         <v>48</v>
       </c>
       <c r="J17" s="13">
         <f t="shared" si="1"/>
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="K17" s="4">
         <f t="shared" si="2"/>
-        <v>88.3</v>
+        <v>90.1</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3076,19 +3084,19 @@
         <f t="shared" si="0"/>
         <v>88.75</v>
       </c>
-      <c r="H19">
-        <v>45</v>
+      <c r="H19" s="18">
+        <v>46</v>
       </c>
       <c r="I19">
         <v>45</v>
       </c>
       <c r="J19" s="13">
         <f t="shared" si="1"/>
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K19" s="4">
         <f t="shared" si="2"/>
-        <v>89.5</v>
+        <v>90.1</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3167,7 +3175,7 @@
         <v>70.699999999999989</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>60</v>
       </c>
@@ -3191,18 +3199,18 @@
         <v>66.25</v>
       </c>
       <c r="H22">
-        <v>32</v>
-      </c>
-      <c r="I22">
-        <v>8</v>
+        <v>40</v>
+      </c>
+      <c r="I22" s="18">
+        <v>16</v>
       </c>
       <c r="J22" s="13">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="K22" s="4">
         <f t="shared" si="2"/>
-        <v>50.5</v>
+        <v>60.1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -3315,19 +3323,19 @@
         <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
-      <c r="H26">
-        <v>42.5</v>
-      </c>
-      <c r="I26">
-        <v>38</v>
+      <c r="H26" s="18">
+        <v>44</v>
+      </c>
+      <c r="I26" s="18">
+        <v>40</v>
       </c>
       <c r="J26" s="13">
         <f t="shared" si="1"/>
-        <v>80.5</v>
+        <v>84</v>
       </c>
       <c r="K26" s="4">
         <f t="shared" si="2"/>
-        <v>83.3</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -3353,19 +3361,19 @@
         <f t="shared" si="0"/>
         <v>78.75</v>
       </c>
-      <c r="H27">
-        <v>37.5</v>
+      <c r="H27" s="18">
+        <v>40</v>
       </c>
       <c r="I27">
         <v>34</v>
       </c>
       <c r="J27" s="13">
         <f t="shared" si="1"/>
-        <v>71.5</v>
+        <v>74</v>
       </c>
       <c r="K27" s="4">
         <f t="shared" si="2"/>
-        <v>74.400000000000006</v>
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -3391,19 +3399,19 @@
         <f t="shared" si="0"/>
         <v>86.25</v>
       </c>
-      <c r="H28">
-        <v>45</v>
+      <c r="H28" s="18">
+        <v>46</v>
       </c>
       <c r="I28">
         <v>39</v>
       </c>
       <c r="J28" s="13">
         <f t="shared" si="1"/>
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K28" s="4">
         <f t="shared" si="2"/>
-        <v>84.9</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -3543,19 +3551,19 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="H32">
-        <v>42.5</v>
+      <c r="H32" s="18">
+        <v>45</v>
       </c>
       <c r="I32">
         <v>45</v>
       </c>
       <c r="J32" s="13">
         <f t="shared" si="1"/>
-        <v>87.5</v>
+        <v>90</v>
       </c>
       <c r="K32" s="4">
         <f t="shared" si="2"/>
-        <v>88.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -3619,19 +3627,19 @@
         <f t="shared" si="0"/>
         <v>86.25</v>
       </c>
-      <c r="H34">
-        <v>35</v>
+      <c r="H34" s="18">
+        <v>37</v>
       </c>
       <c r="I34">
         <v>39</v>
       </c>
       <c r="J34" s="13">
         <f t="shared" si="1"/>
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K34" s="4">
         <f t="shared" si="2"/>
-        <v>78.900000000000006</v>
+        <v>80.099999999999994</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -3771,16 +3779,16 @@
       <c r="H38">
         <v>37.5</v>
       </c>
-      <c r="I38">
-        <v>29</v>
+      <c r="I38" s="18">
+        <v>30</v>
       </c>
       <c r="J38" s="13">
         <f t="shared" si="4"/>
-        <v>66.5</v>
+        <v>67.5</v>
       </c>
       <c r="K38" s="4">
         <f t="shared" si="5"/>
-        <v>69.900000000000006</v>
+        <v>70.5</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -3914,16 +3922,16 @@
       <c r="H42">
         <v>50</v>
       </c>
-      <c r="I42">
-        <v>30</v>
+      <c r="I42" s="18">
+        <v>34</v>
       </c>
       <c r="J42" s="13">
         <f t="shared" si="4"/>
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="K42" s="4">
         <f t="shared" si="5"/>
-        <v>63</v>
+        <v>65.400000000000006</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -3949,19 +3957,19 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H43">
-        <v>45</v>
+      <c r="H43" s="18">
+        <v>46</v>
       </c>
       <c r="I43">
         <v>44</v>
       </c>
       <c r="J43" s="13">
         <f t="shared" si="4"/>
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K43" s="4">
         <f t="shared" si="5"/>
-        <v>89.4</v>
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -4028,16 +4036,16 @@
       <c r="H45">
         <v>37.5</v>
       </c>
-      <c r="I45">
-        <v>12</v>
+      <c r="I45" s="18">
+        <v>14</v>
       </c>
       <c r="J45" s="13">
         <f t="shared" si="4"/>
-        <v>49.5</v>
+        <v>51.5</v>
       </c>
       <c r="K45" s="4">
         <f t="shared" si="5"/>
-        <v>64.2</v>
+        <v>65.400000000000006</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
@@ -4101,19 +4109,19 @@
         <f t="shared" si="3"/>
         <v>77.5</v>
       </c>
-      <c r="H47">
-        <v>22.5</v>
-      </c>
-      <c r="I47">
-        <v>15</v>
+      <c r="H47" s="18">
+        <v>30</v>
+      </c>
+      <c r="I47" s="18">
+        <v>20</v>
       </c>
       <c r="J47" s="13">
         <f t="shared" si="4"/>
-        <v>37.5</v>
+        <v>50</v>
       </c>
       <c r="K47" s="4">
         <f t="shared" si="5"/>
-        <v>53.5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -4139,19 +4147,19 @@
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="H48">
-        <v>42.5</v>
+      <c r="H48" s="18">
+        <v>44</v>
       </c>
       <c r="I48">
         <v>31</v>
       </c>
       <c r="J48" s="13">
         <f t="shared" si="4"/>
-        <v>73.5</v>
+        <v>75</v>
       </c>
       <c r="K48" s="4">
         <f t="shared" si="5"/>
-        <v>74.099999999999994</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
@@ -4180,16 +4188,16 @@
       <c r="H49">
         <v>50</v>
       </c>
-      <c r="I49">
-        <v>36</v>
+      <c r="I49" s="18">
+        <v>38</v>
       </c>
       <c r="J49" s="13">
         <f t="shared" si="4"/>
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="K49" s="4">
         <f t="shared" si="5"/>
-        <v>84.1</v>
+        <v>85.3</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -4364,19 +4372,19 @@
         <f t="shared" si="3"/>
         <v>48.75</v>
       </c>
-      <c r="H54">
-        <v>35</v>
-      </c>
-      <c r="I54">
-        <v>12</v>
+      <c r="H54" s="18">
+        <v>45</v>
+      </c>
+      <c r="I54" s="18">
+        <v>23</v>
       </c>
       <c r="J54" s="13">
         <f t="shared" si="4"/>
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="K54" s="4">
         <f t="shared" si="5"/>
-        <v>47.7</v>
+        <v>60.3</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
@@ -4402,19 +4410,19 @@
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="H55">
-        <v>44</v>
+      <c r="H55" s="18">
+        <v>47</v>
       </c>
       <c r="I55">
         <v>50</v>
       </c>
       <c r="J55" s="13">
         <f t="shared" si="4"/>
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K55" s="4">
         <f t="shared" si="5"/>
-        <v>88.4</v>
+        <v>90.199999999999989</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -4440,19 +4448,19 @@
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="H56">
-        <v>45</v>
+      <c r="H56" s="18">
+        <v>47</v>
       </c>
       <c r="I56">
         <v>47</v>
       </c>
       <c r="J56" s="13">
         <f t="shared" si="4"/>
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K56" s="4">
         <f t="shared" si="5"/>
-        <v>89.199999999999989</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
@@ -4580,19 +4588,19 @@
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="H60">
-        <v>40</v>
-      </c>
-      <c r="I60">
-        <v>12</v>
+      <c r="H60" s="18">
+        <v>45</v>
+      </c>
+      <c r="I60" s="18">
+        <v>25</v>
       </c>
       <c r="J60" s="13">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="K60" s="4">
         <f t="shared" si="5"/>
-        <v>49.2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -4615,19 +4623,19 @@
         <f t="shared" si="3"/>
         <v>53.75</v>
       </c>
-      <c r="H61">
-        <v>22.5</v>
-      </c>
-      <c r="I61">
-        <v>31</v>
+      <c r="H61" s="18">
+        <v>30</v>
+      </c>
+      <c r="I61" s="18">
+        <v>35</v>
       </c>
       <c r="J61" s="13">
         <f t="shared" si="4"/>
-        <v>53.5</v>
+        <v>65</v>
       </c>
       <c r="K61" s="4">
         <f t="shared" si="5"/>
-        <v>53.6</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -4729,19 +4737,19 @@
         <f t="shared" si="3"/>
         <v>66.25</v>
       </c>
-      <c r="H64">
-        <v>26</v>
-      </c>
-      <c r="I64">
-        <v>11</v>
+      <c r="H64" s="18">
+        <v>34</v>
+      </c>
+      <c r="I64" s="18">
+        <v>22</v>
       </c>
       <c r="J64" s="13">
         <f t="shared" si="4"/>
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="K64" s="4">
         <f t="shared" si="5"/>
-        <v>48.7</v>
+        <v>60.1</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
@@ -4808,16 +4816,16 @@
       <c r="H66">
         <v>45</v>
       </c>
-      <c r="I66">
-        <v>33</v>
+      <c r="I66" s="18">
+        <v>34</v>
       </c>
       <c r="J66" s="13">
         <f t="shared" si="4"/>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K66" s="4">
         <f t="shared" si="5"/>
-        <v>79.8</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
@@ -4843,19 +4851,19 @@
         <f t="shared" ref="G67:G98" si="6">D67*0.25+E67*0.5+F67*0.25</f>
         <v>76.25</v>
       </c>
-      <c r="H67">
-        <v>37.5</v>
-      </c>
-      <c r="I67">
-        <v>32</v>
+      <c r="H67" s="18">
+        <v>40</v>
+      </c>
+      <c r="I67" s="18">
+        <v>35</v>
       </c>
       <c r="J67" s="13">
         <f t="shared" ref="J67:J98" si="7">H67+I67</f>
-        <v>69.5</v>
+        <v>75</v>
       </c>
       <c r="K67" s="4">
         <f t="shared" ref="K67:K98" si="8">(G67*0.4)+(J67*0.6)</f>
-        <v>72.199999999999989</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -4916,16 +4924,16 @@
       <c r="H69">
         <v>50</v>
       </c>
-      <c r="I69">
-        <v>42</v>
+      <c r="I69" s="18">
+        <v>44</v>
       </c>
       <c r="J69" s="13">
         <f t="shared" si="7"/>
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="K69" s="4">
         <f t="shared" si="8"/>
-        <v>89.199999999999989</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
@@ -4951,19 +4959,19 @@
         <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="H70">
-        <v>22.5</v>
+      <c r="H70" s="18">
+        <v>25</v>
       </c>
       <c r="I70">
         <v>37</v>
       </c>
       <c r="J70" s="13">
         <f t="shared" si="7"/>
-        <v>59.5</v>
+        <v>62</v>
       </c>
       <c r="K70" s="4">
         <f t="shared" si="8"/>
-        <v>68.699999999999989</v>
+        <v>70.199999999999989</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
@@ -5030,16 +5038,16 @@
       <c r="H72">
         <v>45</v>
       </c>
-      <c r="I72">
-        <v>29</v>
+      <c r="I72" s="18">
+        <v>33</v>
       </c>
       <c r="J72" s="13">
         <f t="shared" si="7"/>
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="K72" s="4">
         <f t="shared" si="8"/>
-        <v>77.900000000000006</v>
+        <v>80.3</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
@@ -5068,16 +5076,16 @@
       <c r="H73">
         <v>50</v>
       </c>
-      <c r="I73">
-        <v>29</v>
+      <c r="I73" s="18">
+        <v>34</v>
       </c>
       <c r="J73" s="13">
         <f t="shared" si="7"/>
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="K73" s="4">
         <f t="shared" si="8"/>
-        <v>82.4</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -5106,16 +5114,16 @@
       <c r="H74">
         <v>45</v>
       </c>
-      <c r="I74">
-        <v>34</v>
+      <c r="I74" s="18">
+        <v>37</v>
       </c>
       <c r="J74" s="13">
         <f t="shared" si="7"/>
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K74" s="4">
         <f t="shared" si="8"/>
-        <v>83.4</v>
+        <v>85.199999999999989</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -5199,19 +5207,19 @@
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="H77">
-        <v>70</v>
-      </c>
-      <c r="I77">
-        <v>24</v>
+      <c r="H77" s="18">
+        <v>45</v>
+      </c>
+      <c r="I77" s="18">
+        <v>35</v>
       </c>
       <c r="J77" s="13">
         <f t="shared" si="7"/>
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="K77" s="4">
         <f t="shared" si="8"/>
-        <v>68.400000000000006</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -5240,16 +5248,16 @@
       <c r="H78">
         <v>45</v>
       </c>
-      <c r="I78">
-        <v>26</v>
+      <c r="I78" s="18">
+        <v>29</v>
       </c>
       <c r="J78" s="13">
         <f t="shared" si="7"/>
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="K78" s="4">
         <f t="shared" si="8"/>
-        <v>78.599999999999994</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
@@ -5345,16 +5353,16 @@
       <c r="H81">
         <v>45</v>
       </c>
-      <c r="I81">
-        <v>40</v>
+      <c r="I81" s="18">
+        <v>44</v>
       </c>
       <c r="J81" s="13">
         <f t="shared" si="7"/>
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="K81" s="4">
         <f t="shared" si="8"/>
-        <v>83</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -5380,19 +5388,19 @@
         <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="H82">
-        <v>45</v>
+      <c r="H82" s="18">
+        <v>48</v>
       </c>
       <c r="I82">
         <v>47</v>
       </c>
       <c r="J82" s="13">
         <f t="shared" si="7"/>
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K82" s="4">
         <f t="shared" si="8"/>
-        <v>88.199999999999989</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
@@ -5444,19 +5452,19 @@
         <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="H84">
-        <v>45</v>
+      <c r="H84" s="18">
+        <v>46</v>
       </c>
       <c r="I84">
         <v>33</v>
       </c>
       <c r="J84" s="13">
         <f t="shared" si="7"/>
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K84" s="4">
         <f t="shared" si="8"/>
-        <v>79.8</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -5669,16 +5677,16 @@
       <c r="H90">
         <v>40</v>
       </c>
-      <c r="I90">
-        <v>26</v>
+      <c r="I90" s="18">
+        <v>28</v>
       </c>
       <c r="J90" s="13">
         <f t="shared" si="7"/>
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K90" s="4">
         <f t="shared" si="8"/>
-        <v>64.599999999999994</v>
+        <v>65.8</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
@@ -5812,16 +5820,16 @@
       <c r="H94">
         <v>50</v>
       </c>
-      <c r="I94">
-        <v>38</v>
+      <c r="I94" s="18">
+        <v>42</v>
       </c>
       <c r="J94" s="13">
         <f t="shared" si="7"/>
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="K94" s="4">
         <f t="shared" si="8"/>
-        <v>87.8</v>
+        <v>90.199999999999989</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
@@ -5915,18 +5923,18 @@
         <v>68.75</v>
       </c>
       <c r="H97">
-        <v>42.5</v>
+        <v>46</v>
       </c>
       <c r="I97">
         <v>34</v>
       </c>
       <c r="J97" s="13">
         <f t="shared" si="7"/>
-        <v>76.5</v>
+        <v>80</v>
       </c>
       <c r="K97" s="4">
         <f t="shared" si="8"/>
-        <v>73.400000000000006</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
@@ -5975,7 +5983,7 @@
         <v>55</v>
       </c>
       <c r="G99" s="9">
-        <f t="shared" ref="G99:G130" si="9">D99*0.25+E99*0.5+F99*0.25</f>
+        <f t="shared" ref="G99:G117" si="9">D99*0.25+E99*0.5+F99*0.25</f>
         <v>75</v>
       </c>
       <c r="H99">
@@ -5985,11 +5993,11 @@
         <v>16</v>
       </c>
       <c r="J99" s="13">
-        <f t="shared" ref="J99:J130" si="10">H99+I99</f>
+        <f t="shared" ref="J99:J117" si="10">H99+I99</f>
         <v>58.5</v>
       </c>
       <c r="K99" s="4">
-        <f t="shared" ref="K99:K130" si="11">(G99*0.4)+(J99*0.6)</f>
+        <f t="shared" ref="K99:K117" si="11">(G99*0.4)+(J99*0.6)</f>
         <v>65.099999999999994</v>
       </c>
     </row>
@@ -6080,19 +6088,19 @@
         <f t="shared" si="9"/>
         <v>71.25</v>
       </c>
-      <c r="H102">
-        <v>25</v>
-      </c>
-      <c r="I102">
-        <v>4</v>
+      <c r="H102" s="18">
+        <v>33</v>
+      </c>
+      <c r="I102" s="18">
+        <v>20</v>
       </c>
       <c r="J102" s="13">
         <f t="shared" si="10"/>
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="K102" s="4">
         <f t="shared" si="11"/>
-        <v>45.9</v>
+        <v>60.3</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
@@ -6153,19 +6161,19 @@
         <f t="shared" si="9"/>
         <v>47.5</v>
       </c>
-      <c r="H104">
-        <v>40</v>
-      </c>
-      <c r="I104">
-        <v>17</v>
+      <c r="H104" s="18">
+        <v>43</v>
+      </c>
+      <c r="I104" s="18">
+        <v>26</v>
       </c>
       <c r="J104" s="13">
         <f t="shared" si="10"/>
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="K104" s="4">
         <f t="shared" si="11"/>
-        <v>53.199999999999996</v>
+        <v>60.4</v>
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.2">
@@ -6191,19 +6199,19 @@
         <f t="shared" si="9"/>
         <v>68.75</v>
       </c>
-      <c r="H105">
-        <v>40</v>
-      </c>
-      <c r="I105">
-        <v>35</v>
+      <c r="H105" s="18">
+        <v>42</v>
+      </c>
+      <c r="I105" s="18">
+        <v>38</v>
       </c>
       <c r="J105" s="13">
         <f t="shared" si="10"/>
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K105" s="4">
         <f t="shared" si="11"/>
-        <v>72.5</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
@@ -6267,19 +6275,19 @@
         <f t="shared" si="9"/>
         <v>75</v>
       </c>
-      <c r="H107">
-        <v>45</v>
+      <c r="H107" s="18">
+        <v>48</v>
       </c>
       <c r="I107">
         <v>36</v>
       </c>
       <c r="J107" s="13">
         <f t="shared" si="10"/>
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="K107" s="4">
         <f t="shared" si="11"/>
-        <v>78.599999999999994</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.2">
@@ -6305,19 +6313,19 @@
         <f t="shared" si="9"/>
         <v>73.75</v>
       </c>
-      <c r="H108">
-        <v>40</v>
+      <c r="H108" s="18">
+        <v>44</v>
       </c>
       <c r="I108">
         <v>32</v>
       </c>
       <c r="J108" s="13">
         <f t="shared" si="10"/>
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="K108" s="4">
         <f t="shared" si="11"/>
-        <v>72.699999999999989</v>
+        <v>75.099999999999994</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.2">
@@ -6378,19 +6386,19 @@
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
-      <c r="H110">
-        <v>22.5</v>
-      </c>
-      <c r="I110">
-        <v>29</v>
+      <c r="H110" s="18">
+        <v>30</v>
+      </c>
+      <c r="I110" s="18">
+        <v>34</v>
       </c>
       <c r="J110" s="13">
         <f t="shared" si="10"/>
-        <v>51.5</v>
+        <v>64</v>
       </c>
       <c r="K110" s="4">
         <f t="shared" si="11"/>
-        <v>52.9</v>
+        <v>60.4</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.2">
@@ -6419,16 +6427,16 @@
       <c r="H111">
         <v>50</v>
       </c>
-      <c r="I111">
-        <v>45</v>
+      <c r="I111" s="18">
+        <v>48</v>
       </c>
       <c r="J111" s="13">
         <f t="shared" si="10"/>
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="K111" s="4">
         <f t="shared" si="11"/>
-        <v>88.5</v>
+        <v>90.3</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.2">
@@ -6591,19 +6599,19 @@
         <f t="shared" si="9"/>
         <v>76.25</v>
       </c>
-      <c r="H116">
-        <v>45</v>
+      <c r="H116" s="18">
+        <v>50</v>
       </c>
       <c r="I116">
         <v>50</v>
       </c>
       <c r="J116" s="13">
         <f t="shared" si="10"/>
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="K116" s="4">
         <f t="shared" si="11"/>
-        <v>87.5</v>
+        <v>90.5</v>
       </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.2">
@@ -6658,7 +6666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D1D592F-937B-D149-BB0B-8ED9164C109C}">
   <dimension ref="A1:A115"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
@@ -7249,11 +7257,604 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAB4FD3-C627-EE4A-87DC-E610ACDA7C75}">
+  <dimension ref="A1:A115"/>
+  <sheetViews>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>61.199999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>61.7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>62.199999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>63.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>64.2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>64.599999999999994</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>65.099999999999994</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>65.900000000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>66.3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>66.900000000000006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>67.3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>67.3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>68.400000000000006</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>68.699999999999989</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>70.3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>70.599999999999994</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>70.699999999999989</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>70.699999999999989</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>70.900000000000006</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>71.599999999999994</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>71.900000000000006</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>72.199999999999989</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>72.199999999999989</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>72.699999999999989</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>73.400000000000006</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>73.599999999999994</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>73.8</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>74.099999999999994</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>74.400000000000006</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>75.699999999999989</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78.599999999999994</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>78.599999999999994</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>79.8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>81.099999999999994</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>81.199999999999989</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>81.400000000000006</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>82.4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>83.3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>83.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>83.4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>83.8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>84.1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>84.9</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>87.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>88.5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>88.699999999999989</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>89.4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>90.1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>90.1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>90.199999999999989</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>90.3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>90.4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>90.4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>90.8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>93.8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>94.199999999999989</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>94.3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A115">
+    <sortCondition ref="A1:A115"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DB2D0D-2955-BA4F-A9C8-09E70872ED6D}">
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Final Scores for Midterms and Finals (Out of 100) - updated 2
</commit_message>
<xml_diff>
--- a/exam_results/Participants_2.xlsx
+++ b/exam_results/Participants_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Desktop/2024_anlp/anlp2024_fall/exam_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF86BED-83BE-9044-BEEC-192F7E4A31B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A399C154-A7DC-B247-BD42-E6AEA6687DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1330,6 +1330,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1339,7 +1340,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2407,10 +2407,10 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2429,15 +2429,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>376</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="H1" s="16" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="H1" s="17" t="s">
         <v>378</v>
       </c>
-      <c r="I1" s="16"/>
+      <c r="I1" s="17"/>
       <c r="J1" s="8" t="s">
         <v>381</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="H6">
         <v>45</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="15">
         <v>29</v>
       </c>
       <c r="J6" s="13">
@@ -2745,7 +2745,7 @@
       <c r="H10">
         <v>42.5</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="15">
         <v>28</v>
       </c>
       <c r="J10" s="13">
@@ -2821,7 +2821,7 @@
       <c r="H12">
         <v>40</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="15">
         <v>48</v>
       </c>
       <c r="J12" s="13">
@@ -2973,7 +2973,7 @@
       <c r="H16">
         <v>42.5</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="15">
         <v>30</v>
       </c>
       <c r="J16" s="13">
@@ -3008,7 +3008,7 @@
         <f t="shared" si="0"/>
         <v>81.25</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="15">
         <v>48</v>
       </c>
       <c r="I17">
@@ -3084,7 +3084,7 @@
         <f t="shared" si="0"/>
         <v>88.75</v>
       </c>
-      <c r="H19" s="18">
+      <c r="H19" s="15">
         <v>46</v>
       </c>
       <c r="I19">
@@ -3201,7 +3201,7 @@
       <c r="H22">
         <v>40</v>
       </c>
-      <c r="I22" s="18">
+      <c r="I22" s="15">
         <v>16</v>
       </c>
       <c r="J22" s="13">
@@ -3286,18 +3286,18 @@
         <v>57.5</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="I25">
         <v>25</v>
       </c>
       <c r="J25" s="13">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="K25" s="4">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>60.199999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -3323,10 +3323,10 @@
         <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
-      <c r="H26" s="18">
+      <c r="H26" s="15">
         <v>44</v>
       </c>
-      <c r="I26" s="18">
+      <c r="I26" s="15">
         <v>40</v>
       </c>
       <c r="J26" s="13">
@@ -3361,7 +3361,7 @@
         <f t="shared" si="0"/>
         <v>78.75</v>
       </c>
-      <c r="H27" s="18">
+      <c r="H27" s="15">
         <v>40</v>
       </c>
       <c r="I27">
@@ -3399,7 +3399,7 @@
         <f t="shared" si="0"/>
         <v>86.25</v>
       </c>
-      <c r="H28" s="18">
+      <c r="H28" s="15">
         <v>46</v>
       </c>
       <c r="I28">
@@ -3551,7 +3551,7 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="H32" s="18">
+      <c r="H32" s="15">
         <v>45</v>
       </c>
       <c r="I32">
@@ -3627,7 +3627,7 @@
         <f t="shared" si="0"/>
         <v>86.25</v>
       </c>
-      <c r="H34" s="18">
+      <c r="H34" s="15">
         <v>37</v>
       </c>
       <c r="I34">
@@ -3779,7 +3779,7 @@
       <c r="H38">
         <v>37.5</v>
       </c>
-      <c r="I38" s="18">
+      <c r="I38" s="15">
         <v>30</v>
       </c>
       <c r="J38" s="13">
@@ -3922,7 +3922,7 @@
       <c r="H42">
         <v>50</v>
       </c>
-      <c r="I42" s="18">
+      <c r="I42" s="15">
         <v>34</v>
       </c>
       <c r="J42" s="13">
@@ -3957,7 +3957,7 @@
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H43" s="18">
+      <c r="H43" s="15">
         <v>46</v>
       </c>
       <c r="I43">
@@ -4036,7 +4036,7 @@
       <c r="H45">
         <v>37.5</v>
       </c>
-      <c r="I45" s="18">
+      <c r="I45" s="15">
         <v>14</v>
       </c>
       <c r="J45" s="13">
@@ -4109,10 +4109,10 @@
         <f t="shared" si="3"/>
         <v>77.5</v>
       </c>
-      <c r="H47" s="18">
+      <c r="H47" s="15">
         <v>30</v>
       </c>
-      <c r="I47" s="18">
+      <c r="I47" s="15">
         <v>20</v>
       </c>
       <c r="J47" s="13">
@@ -4147,7 +4147,7 @@
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="H48" s="18">
+      <c r="H48" s="15">
         <v>44</v>
       </c>
       <c r="I48">
@@ -4188,7 +4188,7 @@
       <c r="H49">
         <v>50</v>
       </c>
-      <c r="I49" s="18">
+      <c r="I49" s="15">
         <v>38</v>
       </c>
       <c r="J49" s="13">
@@ -4372,10 +4372,10 @@
         <f t="shared" si="3"/>
         <v>48.75</v>
       </c>
-      <c r="H54" s="18">
+      <c r="H54" s="15">
         <v>45</v>
       </c>
-      <c r="I54" s="18">
+      <c r="I54" s="15">
         <v>23</v>
       </c>
       <c r="J54" s="13">
@@ -4410,7 +4410,7 @@
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="H55" s="18">
+      <c r="H55" s="15">
         <v>47</v>
       </c>
       <c r="I55">
@@ -4448,7 +4448,7 @@
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="H56" s="18">
+      <c r="H56" s="15">
         <v>47</v>
       </c>
       <c r="I56">
@@ -4588,10 +4588,10 @@
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="H60" s="18">
+      <c r="H60" s="15">
         <v>45</v>
       </c>
-      <c r="I60" s="18">
+      <c r="I60" s="15">
         <v>25</v>
       </c>
       <c r="J60" s="13">
@@ -4623,10 +4623,10 @@
         <f t="shared" si="3"/>
         <v>53.75</v>
       </c>
-      <c r="H61" s="18">
+      <c r="H61" s="15">
         <v>30</v>
       </c>
-      <c r="I61" s="18">
+      <c r="I61" s="15">
         <v>35</v>
       </c>
       <c r="J61" s="13">
@@ -4737,10 +4737,10 @@
         <f t="shared" si="3"/>
         <v>66.25</v>
       </c>
-      <c r="H64" s="18">
+      <c r="H64" s="15">
         <v>34</v>
       </c>
-      <c r="I64" s="18">
+      <c r="I64" s="15">
         <v>22</v>
       </c>
       <c r="J64" s="13">
@@ -4816,7 +4816,7 @@
       <c r="H66">
         <v>45</v>
       </c>
-      <c r="I66" s="18">
+      <c r="I66" s="15">
         <v>34</v>
       </c>
       <c r="J66" s="13">
@@ -4851,10 +4851,10 @@
         <f t="shared" ref="G67:G98" si="6">D67*0.25+E67*0.5+F67*0.25</f>
         <v>76.25</v>
       </c>
-      <c r="H67" s="18">
+      <c r="H67" s="15">
         <v>40</v>
       </c>
-      <c r="I67" s="18">
+      <c r="I67" s="15">
         <v>35</v>
       </c>
       <c r="J67" s="13">
@@ -4924,7 +4924,7 @@
       <c r="H69">
         <v>50</v>
       </c>
-      <c r="I69" s="18">
+      <c r="I69" s="15">
         <v>44</v>
       </c>
       <c r="J69" s="13">
@@ -4959,7 +4959,7 @@
         <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="H70" s="18">
+      <c r="H70" s="15">
         <v>25</v>
       </c>
       <c r="I70">
@@ -5038,7 +5038,7 @@
       <c r="H72">
         <v>45</v>
       </c>
-      <c r="I72" s="18">
+      <c r="I72" s="15">
         <v>33</v>
       </c>
       <c r="J72" s="13">
@@ -5076,7 +5076,7 @@
       <c r="H73">
         <v>50</v>
       </c>
-      <c r="I73" s="18">
+      <c r="I73" s="15">
         <v>34</v>
       </c>
       <c r="J73" s="13">
@@ -5114,7 +5114,7 @@
       <c r="H74">
         <v>45</v>
       </c>
-      <c r="I74" s="18">
+      <c r="I74" s="15">
         <v>37</v>
       </c>
       <c r="J74" s="13">
@@ -5207,10 +5207,10 @@
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="H77" s="18">
+      <c r="H77" s="15">
         <v>45</v>
       </c>
-      <c r="I77" s="18">
+      <c r="I77" s="15">
         <v>35</v>
       </c>
       <c r="J77" s="13">
@@ -5248,7 +5248,7 @@
       <c r="H78">
         <v>45</v>
       </c>
-      <c r="I78" s="18">
+      <c r="I78" s="15">
         <v>29</v>
       </c>
       <c r="J78" s="13">
@@ -5353,7 +5353,7 @@
       <c r="H81">
         <v>45</v>
       </c>
-      <c r="I81" s="18">
+      <c r="I81" s="15">
         <v>44</v>
       </c>
       <c r="J81" s="13">
@@ -5388,7 +5388,7 @@
         <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="H82" s="18">
+      <c r="H82" s="15">
         <v>48</v>
       </c>
       <c r="I82">
@@ -5452,7 +5452,7 @@
         <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="H84" s="18">
+      <c r="H84" s="15">
         <v>46</v>
       </c>
       <c r="I84">
@@ -5677,7 +5677,7 @@
       <c r="H90">
         <v>40</v>
       </c>
-      <c r="I90" s="18">
+      <c r="I90" s="15">
         <v>28</v>
       </c>
       <c r="J90" s="13">
@@ -5820,7 +5820,7 @@
       <c r="H94">
         <v>50</v>
       </c>
-      <c r="I94" s="18">
+      <c r="I94" s="15">
         <v>42</v>
       </c>
       <c r="J94" s="13">
@@ -6088,10 +6088,10 @@
         <f t="shared" si="9"/>
         <v>71.25</v>
       </c>
-      <c r="H102" s="18">
+      <c r="H102" s="15">
         <v>33</v>
       </c>
-      <c r="I102" s="18">
+      <c r="I102" s="15">
         <v>20</v>
       </c>
       <c r="J102" s="13">
@@ -6161,10 +6161,10 @@
         <f t="shared" si="9"/>
         <v>47.5</v>
       </c>
-      <c r="H104" s="18">
+      <c r="H104" s="15">
         <v>43</v>
       </c>
-      <c r="I104" s="18">
+      <c r="I104" s="15">
         <v>26</v>
       </c>
       <c r="J104" s="13">
@@ -6199,10 +6199,10 @@
         <f t="shared" si="9"/>
         <v>68.75</v>
       </c>
-      <c r="H105" s="18">
+      <c r="H105" s="15">
         <v>42</v>
       </c>
-      <c r="I105" s="18">
+      <c r="I105" s="15">
         <v>38</v>
       </c>
       <c r="J105" s="13">
@@ -6275,7 +6275,7 @@
         <f t="shared" si="9"/>
         <v>75</v>
       </c>
-      <c r="H107" s="18">
+      <c r="H107" s="15">
         <v>48</v>
       </c>
       <c r="I107">
@@ -6313,7 +6313,7 @@
         <f t="shared" si="9"/>
         <v>73.75</v>
       </c>
-      <c r="H108" s="18">
+      <c r="H108" s="15">
         <v>44</v>
       </c>
       <c r="I108">
@@ -6386,10 +6386,10 @@
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
-      <c r="H110" s="18">
+      <c r="H110" s="15">
         <v>30</v>
       </c>
-      <c r="I110" s="18">
+      <c r="I110" s="15">
         <v>34</v>
       </c>
       <c r="J110" s="13">
@@ -6427,7 +6427,7 @@
       <c r="H111">
         <v>50</v>
       </c>
-      <c r="I111" s="18">
+      <c r="I111" s="15">
         <v>48</v>
       </c>
       <c r="J111" s="13">
@@ -6599,7 +6599,7 @@
         <f t="shared" si="9"/>
         <v>76.25</v>
       </c>
-      <c r="H116" s="18">
+      <c r="H116" s="15">
         <v>50</v>
       </c>
       <c r="I116">
@@ -7258,592 +7258,943 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAB4FD3-C627-EE4A-87DC-E610ACDA7C75}">
-  <dimension ref="A1:A115"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
+        <v>100</v>
+      </c>
+      <c r="B1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>95</v>
+      </c>
+      <c r="B2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>98</v>
+      </c>
+      <c r="B3">
+        <v>94.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>94.5</v>
+      </c>
+      <c r="B4">
+        <v>94.199999999999989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>98</v>
+      </c>
+      <c r="B5">
+        <v>93.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>98</v>
+      </c>
+      <c r="B6">
+        <v>93.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>95</v>
+      </c>
+      <c r="B7">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>88</v>
+      </c>
+      <c r="B8">
+        <v>90.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>100</v>
+      </c>
+      <c r="B9">
+        <v>90.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>94</v>
+      </c>
+      <c r="B10">
+        <v>90.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>94</v>
+      </c>
+      <c r="B11">
+        <v>90.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>98</v>
+      </c>
+      <c r="B12">
+        <v>90.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>97</v>
+      </c>
+      <c r="B13">
+        <v>90.199999999999989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>92</v>
+      </c>
+      <c r="B14">
+        <v>90.199999999999989</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>96</v>
+      </c>
+      <c r="B15">
+        <v>90.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>91</v>
+      </c>
+      <c r="B16">
+        <v>90.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>90</v>
+      </c>
+      <c r="B17">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>90</v>
+      </c>
+      <c r="B18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>95</v>
+      </c>
+      <c r="B19">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>92</v>
+      </c>
+      <c r="B20">
+        <v>88.699999999999989</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>85</v>
+      </c>
+      <c r="B21">
+        <v>85.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>84</v>
+      </c>
+      <c r="B22">
+        <v>85.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>84</v>
+      </c>
+      <c r="B23">
+        <v>85.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>89</v>
+      </c>
+      <c r="B24">
+        <v>85.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>88</v>
+      </c>
+      <c r="B25">
+        <v>85.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>82</v>
+      </c>
+      <c r="B26">
+        <v>85.199999999999989</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>93</v>
+      </c>
+      <c r="B27">
+        <v>83.8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>79</v>
+      </c>
+      <c r="B28">
+        <v>83.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>74</v>
+      </c>
+      <c r="B29">
+        <v>81.400000000000006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>79.5</v>
+      </c>
+      <c r="B30">
+        <v>81.199999999999989</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>81</v>
+      </c>
+      <c r="B31">
+        <v>81.099999999999994</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>74</v>
+      </c>
+      <c r="B32">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>79</v>
+      </c>
+      <c r="B33">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>74</v>
+      </c>
+      <c r="B34">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>79</v>
+      </c>
+      <c r="B35">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>84</v>
+      </c>
+      <c r="B36">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>78</v>
+      </c>
+      <c r="B37">
+        <v>80.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>76</v>
+      </c>
+      <c r="B38">
+        <v>80.099999999999994</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>70</v>
+      </c>
+      <c r="B39">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>69</v>
+      </c>
+      <c r="B40">
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>74</v>
+      </c>
+      <c r="B41">
+        <v>75.900000000000006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>67</v>
+      </c>
+      <c r="B42">
+        <v>75.699999999999989</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>75</v>
+      </c>
+      <c r="B43">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>72.5</v>
+      </c>
+      <c r="B44">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>80</v>
+      </c>
+      <c r="B45">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>80</v>
+      </c>
+      <c r="B46">
+        <v>75.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>74</v>
+      </c>
+      <c r="B47">
+        <v>75.400000000000006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>76</v>
+      </c>
+      <c r="B48">
+        <v>75.099999999999994</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>72.5</v>
+      </c>
+      <c r="B49">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>75</v>
+      </c>
+      <c r="B50">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>65</v>
+      </c>
+      <c r="B51">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>67.5</v>
+      </c>
+      <c r="B52">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>72</v>
+      </c>
+      <c r="B53">
+        <v>72.199999999999989</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>69</v>
+      </c>
+      <c r="B54">
+        <v>71.900000000000006</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>66</v>
+      </c>
+      <c r="B55">
+        <v>71.599999999999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>65</v>
+      </c>
+      <c r="B56">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>64</v>
+      </c>
+      <c r="B57">
+        <v>70.900000000000006</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>72</v>
+      </c>
+      <c r="B58">
+        <v>70.699999999999989</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>67</v>
+      </c>
+      <c r="B59">
+        <v>70.699999999999989</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>63.5</v>
+      </c>
+      <c r="B60">
+        <v>70.599999999999994</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>67.5</v>
+      </c>
+      <c r="B61">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>66.5</v>
+      </c>
+      <c r="B62">
+        <v>70.400000000000006</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>70.5</v>
+      </c>
+      <c r="B63">
+        <v>70.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>70.199999999999989</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>67.5</v>
+      </c>
+      <c r="B65">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>60.5</v>
+      </c>
+      <c r="B66">
+        <v>67.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>58</v>
+      </c>
+      <c r="B67">
+        <v>67.3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>71.5</v>
+      </c>
+      <c r="B68">
+        <v>66.900000000000006</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>66.3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>62.5</v>
+      </c>
+      <c r="B70">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>51.5</v>
+      </c>
+      <c r="B71">
+        <v>65.900000000000006</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>68</v>
+      </c>
+      <c r="B72">
+        <v>65.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>84</v>
+      </c>
+      <c r="B73">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>51.5</v>
+      </c>
+      <c r="B74">
+        <v>65.400000000000006</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>58.5</v>
+      </c>
+      <c r="B75">
+        <v>65.099999999999994</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>65.5</v>
+      </c>
+      <c r="B76">
+        <v>63.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>57</v>
+      </c>
+      <c r="B77">
+        <v>62.199999999999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>52</v>
+      </c>
+      <c r="B78">
+        <v>61.7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B79" t="e">
+        <f>SUM(#REF!)</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>55</v>
+      </c>
+      <c r="B80">
+        <v>61.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>82</v>
+      </c>
+      <c r="B81">
+        <v>61.199999999999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>70</v>
+      </c>
+      <c r="B82">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>50</v>
+      </c>
+      <c r="B83">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>65</v>
+      </c>
+      <c r="B84">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>50</v>
+      </c>
+      <c r="B85">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>69</v>
+      </c>
+      <c r="B86">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>64</v>
+      </c>
+      <c r="B87">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>64</v>
+      </c>
+      <c r="B88">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>68</v>
+      </c>
+      <c r="B89">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>53</v>
+      </c>
+      <c r="B90">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>56</v>
+      </c>
+      <c r="B91">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>56</v>
+      </c>
+      <c r="B92">
+        <v>60.1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>50</v>
+      </c>
+      <c r="B93">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>70</v>
+      </c>
+      <c r="B94">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>80</v>
+      </c>
+      <c r="B95">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>40</v>
+      </c>
+      <c r="B96">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>25</v>
+      </c>
+      <c r="B97">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>36.5</v>
+      </c>
+      <c r="B98">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>30</v>
+      </c>
+      <c r="B99">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>5</v>
+      </c>
+      <c r="B100">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>3</v>
+      </c>
+      <c r="B101">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>14</v>
+      </c>
+      <c r="B102">
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="B103">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="B104">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B105">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>2</v>
+      </c>
+      <c r="B106">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="B107">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="B108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B109">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>26.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>27.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>35.9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>60.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>60.1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>60.3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>60.3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>60.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>60.4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>60.4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>61.199999999999996</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>61.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>61.7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>62.199999999999996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>63.8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>64.2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>64.599999999999994</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>65.099999999999994</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>65.400000000000006</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>65.900000000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>66.3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>66.900000000000006</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>67.3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>67.3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>68.400000000000006</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>68.699999999999989</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>70.3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>70.400000000000006</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>70.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>70.599999999999994</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>70.699999999999989</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>70.699999999999989</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>70.900000000000006</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>71.599999999999994</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>71.900000000000006</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>72.199999999999989</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>72.199999999999989</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>72.5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>72.699999999999989</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>73.400000000000006</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>73.599999999999994</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>73.8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>74.099999999999994</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>74.400000000000006</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>75.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>75.699999999999989</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>77.900000000000006</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>77.900000000000006</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>78.5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>78.599999999999994</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>78.599999999999994</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>78.900000000000006</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>79.8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>79.8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>80.400000000000006</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>81.099999999999994</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>81.199999999999989</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>81.400000000000006</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>82.4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>83.3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>83.4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>83.4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>83.8</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>84.1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>84.9</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>87.8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>88.5</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>88.699999999999989</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>89.4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>90.1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <v>90.1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <v>90.199999999999989</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104">
-        <v>90.3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105">
-        <v>90.4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106">
-        <v>90.4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <v>90.5</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <v>90.8</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>93.3</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>93.8</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>94.199999999999989</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>94.3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>98</v>
+        <v>0</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>0</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A115">
-    <sortCondition ref="A1:A115"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B138">
+    <sortCondition descending="1" ref="B23:B138"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8211,21 +8562,21 @@
       <c r="A31" t="s">
         <v>371</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="18">
         <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E32" s="17"/>
+      <c r="E32" s="18"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E33" s="17"/>
+      <c r="E33" s="18"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E34" s="17"/>
+      <c r="E34" s="18"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E35" s="17"/>
+      <c r="E35" s="18"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">

</xml_diff>

<commit_message>
Final Scores for Midterms and Finals - updated 2 - Presantations minor updates
</commit_message>
<xml_diff>
--- a/exam_results/Participants_2.xlsx
+++ b/exam_results/Participants_2.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/can.kara/Desktop/2024_anlp/anlp2024_fall/exam_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A399C154-A7DC-B247-BD42-E6AEA6687DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4419444-9694-C248-B0E0-87F937AF089D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$H$1:$H$117</definedName>
@@ -1277,13 +1276,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1306,32 +1305,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2407,10 +2406,10 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2418,14 +2417,14 @@
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
-    <col min="7" max="7" width="11.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="11.5" style="14" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" customWidth="1"/>
     <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="33.33203125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="23.5" style="4" customWidth="1"/>
+    <col min="10" max="10" width="40.83203125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="23.5" style="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.2">
@@ -2464,19 +2463,19 @@
       <c r="F2" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="12" t="s">
         <v>350</v>
       </c>
     </row>
@@ -2499,7 +2498,7 @@
       <c r="F3">
         <v>95</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="14">
         <f t="shared" ref="G3:G34" si="0">D3*0.25+E3*0.5+F3*0.25</f>
         <v>76.25</v>
       </c>
@@ -2509,11 +2508,11 @@
       <c r="I3">
         <v>7</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="10">
         <f t="shared" ref="J3:J34" si="1">H3+I3</f>
         <v>52</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="13">
         <f t="shared" ref="K3:K34" si="2">(G3*0.4)+(J3*0.6)</f>
         <v>61.7</v>
       </c>
@@ -2537,7 +2536,7 @@
       <c r="F4">
         <v>95</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="14">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
@@ -2547,11 +2546,11 @@
       <c r="I4">
         <v>5</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="10">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="13">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
@@ -2569,18 +2568,18 @@
       <c r="E5">
         <v>75</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="14">
         <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="13">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
@@ -2604,21 +2603,21 @@
       <c r="F6">
         <v>95</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="14">
         <f t="shared" si="0"/>
         <v>77.5</v>
       </c>
       <c r="H6">
         <v>45</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="7">
         <v>29</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="10">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="13">
         <f t="shared" si="2"/>
         <v>75.400000000000006</v>
       </c>
@@ -2642,23 +2641,23 @@
       <c r="F7">
         <v>95</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="14">
         <f t="shared" si="0"/>
         <v>93.75</v>
       </c>
       <c r="H7">
-        <v>47.5</v>
+        <v>49</v>
       </c>
       <c r="I7">
-        <v>47</v>
-      </c>
-      <c r="J7" s="13">
+        <v>48</v>
+      </c>
+      <c r="J7" s="10">
         <f t="shared" si="1"/>
-        <v>94.5</v>
-      </c>
-      <c r="K7" s="4">
+        <v>97</v>
+      </c>
+      <c r="K7" s="13">
         <f t="shared" si="2"/>
-        <v>94.199999999999989</v>
+        <v>95.699999999999989</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2671,18 +2670,18 @@
       <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2700,7 +2699,7 @@
       <c r="E9">
         <v>70</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="14">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
@@ -2710,11 +2709,11 @@
       <c r="I9">
         <v>14</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="10">
         <f t="shared" si="1"/>
         <v>36.5</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="13">
         <f t="shared" si="2"/>
         <v>35.9</v>
       </c>
@@ -2738,21 +2737,21 @@
       <c r="F10">
         <v>55</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="14">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
       <c r="H10">
         <v>42.5</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="7">
         <v>28</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="10">
         <f t="shared" si="1"/>
         <v>70.5</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="13">
         <f t="shared" si="2"/>
         <v>70.3</v>
       </c>
@@ -2776,7 +2775,7 @@
       <c r="F11">
         <v>90</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="14">
         <f t="shared" si="0"/>
         <v>91.25</v>
       </c>
@@ -2786,11 +2785,11 @@
       <c r="I11">
         <v>24</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="10">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="13">
         <f t="shared" si="2"/>
         <v>77.900000000000006</v>
       </c>
@@ -2814,21 +2813,21 @@
       <c r="F12">
         <v>100</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="14">
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
       <c r="H12">
         <v>40</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="7">
         <v>48</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="10">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="13">
         <f t="shared" si="2"/>
         <v>90.8</v>
       </c>
@@ -2852,7 +2851,7 @@
       <c r="F13">
         <v>80</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="14">
         <f t="shared" si="0"/>
         <v>77.5</v>
       </c>
@@ -2862,11 +2861,11 @@
       <c r="I13">
         <v>23</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="10">
         <f t="shared" si="1"/>
         <v>60.5</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="13">
         <f t="shared" si="2"/>
         <v>67.3</v>
       </c>
@@ -2890,7 +2889,7 @@
       <c r="F14">
         <v>55</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="14">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
@@ -2900,11 +2899,11 @@
       <c r="I14">
         <v>48</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="10">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="13">
         <f t="shared" si="2"/>
         <v>83.8</v>
       </c>
@@ -2928,7 +2927,7 @@
       <c r="F15">
         <v>100</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="14">
         <f t="shared" si="0"/>
         <v>86.25</v>
       </c>
@@ -2938,11 +2937,11 @@
       <c r="I15">
         <v>50</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="10">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="13">
         <f t="shared" si="2"/>
         <v>93.3</v>
       </c>
@@ -2966,21 +2965,21 @@
       <c r="F16">
         <v>55</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="14">
         <f t="shared" si="0"/>
         <v>78.75</v>
       </c>
       <c r="H16">
         <v>42.5</v>
       </c>
-      <c r="I16" s="15">
+      <c r="I16" s="7">
         <v>30</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="10">
         <f t="shared" si="1"/>
         <v>72.5</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="13">
         <f t="shared" si="2"/>
         <v>75</v>
       </c>
@@ -3004,21 +3003,21 @@
       <c r="F17">
         <v>95</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G17" s="14">
         <f t="shared" si="0"/>
         <v>81.25</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="7">
         <v>48</v>
       </c>
       <c r="I17">
         <v>48</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="10">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="13">
         <f t="shared" si="2"/>
         <v>90.1</v>
       </c>
@@ -3042,7 +3041,7 @@
       <c r="F18">
         <v>100</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="14">
         <f t="shared" si="0"/>
         <v>88.75</v>
       </c>
@@ -3052,11 +3051,11 @@
       <c r="I18">
         <v>48</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="10">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="13">
         <f t="shared" si="2"/>
         <v>94.3</v>
       </c>
@@ -3080,21 +3079,21 @@
       <c r="F19">
         <v>95</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="14">
         <f t="shared" si="0"/>
         <v>88.75</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H19" s="7">
         <v>46</v>
       </c>
       <c r="I19">
         <v>45</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="10">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="13">
         <f t="shared" si="2"/>
         <v>90.1</v>
       </c>
@@ -3118,7 +3117,7 @@
       <c r="F20">
         <v>95</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="14">
         <f t="shared" si="0"/>
         <v>72.5</v>
       </c>
@@ -3128,11 +3127,11 @@
       <c r="I20">
         <v>27</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="10">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="13">
         <f t="shared" si="2"/>
         <v>72.199999999999989</v>
       </c>
@@ -3156,7 +3155,7 @@
       <c r="F21">
         <v>95</v>
       </c>
-      <c r="G21" s="9">
+      <c r="G21" s="14">
         <f t="shared" si="0"/>
         <v>68.75</v>
       </c>
@@ -3166,11 +3165,11 @@
       <c r="I21">
         <v>27</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="10">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="13">
         <f t="shared" si="2"/>
         <v>70.699999999999989</v>
       </c>
@@ -3194,21 +3193,21 @@
       <c r="F22">
         <v>50</v>
       </c>
-      <c r="G22" s="9">
+      <c r="G22" s="14">
         <f t="shared" si="0"/>
         <v>66.25</v>
       </c>
       <c r="H22">
         <v>40</v>
       </c>
-      <c r="I22" s="15">
+      <c r="I22" s="7">
         <v>16</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="10">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="13">
         <f t="shared" si="2"/>
         <v>60.1</v>
       </c>
@@ -3223,18 +3222,18 @@
       <c r="C23" t="s">
         <v>65</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3249,18 +3248,18 @@
       <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3281,7 +3280,7 @@
       <c r="F25">
         <v>80</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="14">
         <f t="shared" si="0"/>
         <v>57.5</v>
       </c>
@@ -3291,11 +3290,11 @@
       <c r="I25">
         <v>25</v>
       </c>
-      <c r="J25" s="13">
+      <c r="J25" s="10">
         <f t="shared" si="1"/>
         <v>62</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="13">
         <f t="shared" si="2"/>
         <v>60.199999999999996</v>
       </c>
@@ -3319,21 +3318,21 @@
       <c r="F26">
         <v>100</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="14">
         <f t="shared" si="0"/>
         <v>87.5</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="7">
         <v>44</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="7">
         <v>40</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="10">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="13">
         <f t="shared" si="2"/>
         <v>85.4</v>
       </c>
@@ -3357,21 +3356,21 @@
       <c r="F27">
         <v>85</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="14">
         <f t="shared" si="0"/>
         <v>78.75</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="7">
         <v>40</v>
       </c>
       <c r="I27">
         <v>34</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="10">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="13">
         <f t="shared" si="2"/>
         <v>75.900000000000006</v>
       </c>
@@ -3395,21 +3394,21 @@
       <c r="F28">
         <v>95</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="14">
         <f t="shared" si="0"/>
         <v>86.25</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="7">
         <v>46</v>
       </c>
       <c r="I28">
         <v>39</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="10">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="13">
         <f t="shared" si="2"/>
         <v>85.5</v>
       </c>
@@ -3433,7 +3432,7 @@
       <c r="F29">
         <v>85</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="14">
         <f t="shared" si="0"/>
         <v>76.25</v>
       </c>
@@ -3443,11 +3442,11 @@
       <c r="I29">
         <v>22</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="10">
         <f t="shared" si="1"/>
         <v>67</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="13">
         <f t="shared" si="2"/>
         <v>70.699999999999989</v>
       </c>
@@ -3471,7 +3470,7 @@
       <c r="F30">
         <v>95</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="14">
         <f t="shared" si="0"/>
         <v>76.25</v>
       </c>
@@ -3481,11 +3480,11 @@
       <c r="I30">
         <v>24</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="10">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30" s="13">
         <f t="shared" si="2"/>
         <v>71.900000000000006</v>
       </c>
@@ -3509,7 +3508,7 @@
       <c r="F31">
         <v>95</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="14">
         <f t="shared" si="0"/>
         <v>81.25</v>
       </c>
@@ -3519,11 +3518,11 @@
       <c r="I31">
         <v>31</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="10">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K31" s="13">
         <f t="shared" si="2"/>
         <v>81.099999999999994</v>
       </c>
@@ -3547,21 +3546,21 @@
       <c r="F32">
         <v>90</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="14">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="7">
         <v>45</v>
       </c>
       <c r="I32">
         <v>45</v>
       </c>
-      <c r="J32" s="13">
+      <c r="J32" s="10">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K32" s="13">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
@@ -3585,7 +3584,7 @@
       <c r="F33">
         <v>80</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="14">
         <f t="shared" si="0"/>
         <v>71.25</v>
       </c>
@@ -3595,11 +3594,11 @@
       <c r="I33">
         <v>30</v>
       </c>
-      <c r="J33" s="13">
+      <c r="J33" s="10">
         <f t="shared" si="1"/>
         <v>55</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K33" s="13">
         <f t="shared" si="2"/>
         <v>61.5</v>
       </c>
@@ -3623,21 +3622,21 @@
       <c r="F34">
         <v>85</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="14">
         <f t="shared" si="0"/>
         <v>86.25</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H34" s="7">
         <v>37</v>
       </c>
       <c r="I34">
         <v>39</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="10">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="13">
         <f t="shared" si="2"/>
         <v>80.099999999999994</v>
       </c>
@@ -3661,7 +3660,7 @@
       <c r="F35">
         <v>80</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="14">
         <f t="shared" ref="G35:G66" si="3">D35*0.25+E35*0.5+F35*0.25</f>
         <v>73.75</v>
       </c>
@@ -3671,11 +3670,11 @@
       <c r="I35">
         <v>30</v>
       </c>
-      <c r="J35" s="13">
+      <c r="J35" s="10">
         <f t="shared" ref="J35:J66" si="4">H35+I35</f>
         <v>67.5</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K35" s="13">
         <f t="shared" ref="K35:K66" si="5">(G35*0.4)+(J35*0.6)</f>
         <v>70</v>
       </c>
@@ -3699,7 +3698,7 @@
       <c r="F36">
         <v>100</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="14">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
@@ -3709,11 +3708,11 @@
       <c r="I36">
         <v>29</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="10">
         <f t="shared" si="4"/>
         <v>74</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36" s="13">
         <f t="shared" si="5"/>
         <v>80.400000000000006</v>
       </c>
@@ -3734,7 +3733,7 @@
       <c r="F37">
         <v>60</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="14">
         <f t="shared" si="3"/>
         <v>62.5</v>
       </c>
@@ -3744,11 +3743,11 @@
       <c r="I37">
         <v>5</v>
       </c>
-      <c r="J37" s="13">
+      <c r="J37" s="10">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37" s="13">
         <f t="shared" si="5"/>
         <v>28</v>
       </c>
@@ -3772,21 +3771,21 @@
       <c r="F38">
         <v>100</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="14">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="H38">
         <v>37.5</v>
       </c>
-      <c r="I38" s="15">
+      <c r="I38" s="7">
         <v>30</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="10">
         <f t="shared" si="4"/>
         <v>67.5</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="13">
         <f t="shared" si="5"/>
         <v>70.5</v>
       </c>
@@ -3810,7 +3809,7 @@
       <c r="F39">
         <v>100</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="14">
         <f t="shared" si="3"/>
         <v>95</v>
       </c>
@@ -3820,11 +3819,11 @@
       <c r="I39">
         <v>45</v>
       </c>
-      <c r="J39" s="13">
+      <c r="J39" s="10">
         <f t="shared" si="4"/>
         <v>95</v>
       </c>
-      <c r="K39" s="4">
+      <c r="K39" s="13">
         <f t="shared" si="5"/>
         <v>95</v>
       </c>
@@ -3842,7 +3841,7 @@
       <c r="E40">
         <v>95</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="14">
         <f t="shared" si="3"/>
         <v>47.5</v>
       </c>
@@ -3852,11 +3851,11 @@
       <c r="I40">
         <v>30</v>
       </c>
-      <c r="J40" s="13">
+      <c r="J40" s="10">
         <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="K40" s="4">
+      <c r="K40" s="13">
         <f t="shared" si="5"/>
         <v>61</v>
       </c>
@@ -3880,7 +3879,7 @@
       <c r="F41">
         <v>90</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="14">
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
@@ -3890,11 +3889,11 @@
       <c r="I41">
         <v>25</v>
       </c>
-      <c r="J41" s="13">
+      <c r="J41" s="10">
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="K41" s="4">
+      <c r="K41" s="13">
         <f t="shared" si="5"/>
         <v>73</v>
       </c>
@@ -3915,21 +3914,21 @@
       <c r="F42">
         <v>0</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="14">
         <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
       <c r="H42">
         <v>50</v>
       </c>
-      <c r="I42" s="15">
+      <c r="I42" s="7">
         <v>34</v>
       </c>
-      <c r="J42" s="13">
+      <c r="J42" s="10">
         <f t="shared" si="4"/>
         <v>84</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="13">
         <f t="shared" si="5"/>
         <v>65.400000000000006</v>
       </c>
@@ -3953,21 +3952,21 @@
       <c r="F43">
         <v>90</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="14">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H43" s="7">
         <v>46</v>
       </c>
       <c r="I43">
         <v>44</v>
       </c>
-      <c r="J43" s="13">
+      <c r="J43" s="10">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
-      <c r="K43" s="4">
+      <c r="K43" s="13">
         <f t="shared" si="5"/>
         <v>90</v>
       </c>
@@ -3991,7 +3990,7 @@
       <c r="F44">
         <v>85</v>
       </c>
-      <c r="G44" s="9">
+      <c r="G44" s="14">
         <f t="shared" si="3"/>
         <v>88.75</v>
       </c>
@@ -4001,11 +4000,11 @@
       <c r="I44">
         <v>22</v>
       </c>
-      <c r="J44" s="13">
+      <c r="J44" s="10">
         <f t="shared" si="4"/>
         <v>67</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K44" s="13">
         <f t="shared" si="5"/>
         <v>75.699999999999989</v>
       </c>
@@ -4029,21 +4028,21 @@
       <c r="F45">
         <v>100</v>
       </c>
-      <c r="G45" s="9">
+      <c r="G45" s="14">
         <f t="shared" si="3"/>
         <v>86.25</v>
       </c>
       <c r="H45">
         <v>37.5</v>
       </c>
-      <c r="I45" s="15">
+      <c r="I45" s="7">
         <v>14</v>
       </c>
-      <c r="J45" s="13">
+      <c r="J45" s="10">
         <f t="shared" si="4"/>
         <v>51.5</v>
       </c>
-      <c r="K45" s="4">
+      <c r="K45" s="13">
         <f t="shared" si="5"/>
         <v>65.400000000000006</v>
       </c>
@@ -4059,7 +4058,7 @@
         <v>134</v>
       </c>
       <c r="D46">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E46">
         <v>75</v>
@@ -4067,9 +4066,9 @@
       <c r="F46">
         <v>95</v>
       </c>
-      <c r="G46" s="9">
+      <c r="G46" s="14">
         <f t="shared" si="3"/>
-        <v>81.25</v>
+        <v>82.5</v>
       </c>
       <c r="H46">
         <v>37.5</v>
@@ -4077,13 +4076,13 @@
       <c r="I46">
         <v>30</v>
       </c>
-      <c r="J46" s="13">
+      <c r="J46" s="10">
         <f t="shared" si="4"/>
         <v>67.5</v>
       </c>
-      <c r="K46" s="4">
+      <c r="K46" s="13">
         <f t="shared" si="5"/>
-        <v>73</v>
+        <v>73.5</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -4105,21 +4104,21 @@
       <c r="F47">
         <v>60</v>
       </c>
-      <c r="G47" s="9">
+      <c r="G47" s="14">
         <f t="shared" si="3"/>
         <v>77.5</v>
       </c>
-      <c r="H47" s="15">
+      <c r="H47" s="7">
         <v>30</v>
       </c>
-      <c r="I47" s="15">
+      <c r="I47" s="7">
         <v>20</v>
       </c>
-      <c r="J47" s="13">
+      <c r="J47" s="10">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="K47" s="4">
+      <c r="K47" s="13">
         <f t="shared" si="5"/>
         <v>61</v>
       </c>
@@ -4143,21 +4142,21 @@
       <c r="F48">
         <v>55</v>
       </c>
-      <c r="G48" s="9">
+      <c r="G48" s="14">
         <f t="shared" si="3"/>
         <v>75</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H48" s="7">
         <v>44</v>
       </c>
       <c r="I48">
         <v>31</v>
       </c>
-      <c r="J48" s="13">
+      <c r="J48" s="10">
         <f t="shared" si="4"/>
         <v>75</v>
       </c>
-      <c r="K48" s="4">
+      <c r="K48" s="13">
         <f t="shared" si="5"/>
         <v>75</v>
       </c>
@@ -4181,21 +4180,21 @@
       <c r="F49">
         <v>90</v>
       </c>
-      <c r="G49" s="9">
+      <c r="G49" s="14">
         <f t="shared" si="3"/>
         <v>81.25</v>
       </c>
       <c r="H49">
         <v>50</v>
       </c>
-      <c r="I49" s="15">
+      <c r="I49" s="7">
         <v>38</v>
       </c>
-      <c r="J49" s="13">
+      <c r="J49" s="10">
         <f t="shared" si="4"/>
         <v>88</v>
       </c>
-      <c r="K49" s="4">
+      <c r="K49" s="13">
         <f t="shared" si="5"/>
         <v>85.3</v>
       </c>
@@ -4219,7 +4218,7 @@
       <c r="F50">
         <v>80</v>
       </c>
-      <c r="G50" s="9">
+      <c r="G50" s="14">
         <f t="shared" si="3"/>
         <v>81.25</v>
       </c>
@@ -4229,11 +4228,11 @@
       <c r="I50">
         <v>19</v>
       </c>
-      <c r="J50" s="13">
+      <c r="J50" s="10">
         <f t="shared" si="4"/>
         <v>64</v>
       </c>
-      <c r="K50" s="4">
+      <c r="K50" s="13">
         <f t="shared" si="5"/>
         <v>70.900000000000006</v>
       </c>
@@ -4257,7 +4256,7 @@
       <c r="F51">
         <v>85</v>
       </c>
-      <c r="G51" s="9">
+      <c r="G51" s="14">
         <f t="shared" si="3"/>
         <v>63.75</v>
       </c>
@@ -4267,11 +4266,11 @@
       <c r="I51">
         <v>43</v>
       </c>
-      <c r="J51" s="13">
+      <c r="J51" s="10">
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="K51" s="4">
+      <c r="K51" s="13">
         <f t="shared" si="5"/>
         <v>66.3</v>
       </c>
@@ -4295,7 +4294,7 @@
       <c r="F52">
         <v>55</v>
       </c>
-      <c r="G52" s="9">
+      <c r="G52" s="14">
         <f t="shared" si="3"/>
         <v>60</v>
       </c>
@@ -4305,11 +4304,11 @@
       <c r="I52">
         <v>29</v>
       </c>
-      <c r="J52" s="13">
+      <c r="J52" s="10">
         <f t="shared" si="4"/>
         <v>71.5</v>
       </c>
-      <c r="K52" s="4">
+      <c r="K52" s="13">
         <f t="shared" si="5"/>
         <v>66.900000000000006</v>
       </c>
@@ -4333,7 +4332,7 @@
       <c r="F53">
         <v>60</v>
       </c>
-      <c r="G53" s="9">
+      <c r="G53" s="14">
         <f t="shared" si="3"/>
         <v>70</v>
       </c>
@@ -4343,11 +4342,11 @@
       <c r="I53">
         <v>17</v>
       </c>
-      <c r="J53" s="13">
+      <c r="J53" s="10">
         <f t="shared" si="4"/>
         <v>57</v>
       </c>
-      <c r="K53" s="4">
+      <c r="K53" s="13">
         <f t="shared" si="5"/>
         <v>62.199999999999996</v>
       </c>
@@ -4368,21 +4367,21 @@
       <c r="F54">
         <v>55</v>
       </c>
-      <c r="G54" s="9">
+      <c r="G54" s="14">
         <f t="shared" si="3"/>
         <v>48.75</v>
       </c>
-      <c r="H54" s="15">
+      <c r="H54" s="7">
         <v>45</v>
       </c>
-      <c r="I54" s="15">
+      <c r="I54" s="7">
         <v>23</v>
       </c>
-      <c r="J54" s="13">
+      <c r="J54" s="10">
         <f t="shared" si="4"/>
         <v>68</v>
       </c>
-      <c r="K54" s="4">
+      <c r="K54" s="13">
         <f t="shared" si="5"/>
         <v>60.3</v>
       </c>
@@ -4406,21 +4405,21 @@
       <c r="F55">
         <v>100</v>
       </c>
-      <c r="G55" s="9">
+      <c r="G55" s="14">
         <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="H55" s="15">
+      <c r="H55" s="7">
         <v>47</v>
       </c>
       <c r="I55">
         <v>50</v>
       </c>
-      <c r="J55" s="13">
+      <c r="J55" s="10">
         <f t="shared" si="4"/>
         <v>97</v>
       </c>
-      <c r="K55" s="4">
+      <c r="K55" s="13">
         <f t="shared" si="5"/>
         <v>90.199999999999989</v>
       </c>
@@ -4444,21 +4443,21 @@
       <c r="F56">
         <v>100</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G56" s="14">
         <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="H56" s="15">
+      <c r="H56" s="7">
         <v>47</v>
       </c>
       <c r="I56">
         <v>47</v>
       </c>
-      <c r="J56" s="13">
+      <c r="J56" s="10">
         <f t="shared" si="4"/>
         <v>94</v>
       </c>
-      <c r="K56" s="4">
+      <c r="K56" s="13">
         <f t="shared" si="5"/>
         <v>90.4</v>
       </c>
@@ -4473,18 +4472,18 @@
       <c r="C57" t="s">
         <v>167</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
-      <c r="J57" s="13">
+      <c r="J57" s="10">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K57" s="4">
+      <c r="K57" s="13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -4508,7 +4507,7 @@
       <c r="F58">
         <v>85</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G58" s="14">
         <f t="shared" si="3"/>
         <v>91.25</v>
       </c>
@@ -4518,11 +4517,11 @@
       <c r="I58">
         <v>25</v>
       </c>
-      <c r="J58" s="13">
+      <c r="J58" s="10">
         <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="K58" s="4">
+      <c r="K58" s="13">
         <f t="shared" si="5"/>
         <v>78.5</v>
       </c>
@@ -4546,7 +4545,7 @@
       <c r="F59">
         <v>55</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G59" s="14">
         <f t="shared" si="3"/>
         <v>71.25</v>
       </c>
@@ -4556,11 +4555,11 @@
       <c r="I59">
         <v>20</v>
       </c>
-      <c r="J59" s="13">
+      <c r="J59" s="10">
         <f t="shared" si="4"/>
         <v>62.5</v>
       </c>
-      <c r="K59" s="4">
+      <c r="K59" s="13">
         <f t="shared" si="5"/>
         <v>66</v>
       </c>
@@ -4584,21 +4583,21 @@
       <c r="F60">
         <v>55</v>
       </c>
-      <c r="G60" s="9">
+      <c r="G60" s="14">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="H60" s="15">
+      <c r="H60" s="7">
         <v>45</v>
       </c>
-      <c r="I60" s="15">
+      <c r="I60" s="7">
         <v>25</v>
       </c>
-      <c r="J60" s="13">
+      <c r="J60" s="10">
         <f t="shared" si="4"/>
         <v>70</v>
       </c>
-      <c r="K60" s="4">
+      <c r="K60" s="13">
         <f t="shared" si="5"/>
         <v>60</v>
       </c>
@@ -4619,21 +4618,21 @@
       <c r="F61">
         <v>85</v>
       </c>
-      <c r="G61" s="9">
+      <c r="G61" s="14">
         <f t="shared" si="3"/>
         <v>53.75</v>
       </c>
-      <c r="H61" s="15">
+      <c r="H61" s="7">
         <v>30</v>
       </c>
-      <c r="I61" s="15">
+      <c r="I61" s="7">
         <v>35</v>
       </c>
-      <c r="J61" s="13">
+      <c r="J61" s="10">
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
-      <c r="K61" s="4">
+      <c r="K61" s="13">
         <f t="shared" si="5"/>
         <v>60.5</v>
       </c>
@@ -4657,7 +4656,7 @@
       <c r="F62">
         <v>95</v>
       </c>
-      <c r="G62" s="9">
+      <c r="G62" s="14">
         <f t="shared" si="3"/>
         <v>83.75</v>
       </c>
@@ -4667,11 +4666,11 @@
       <c r="I62">
         <v>47</v>
       </c>
-      <c r="J62" s="13">
+      <c r="J62" s="10">
         <f t="shared" si="4"/>
         <v>92</v>
       </c>
-      <c r="K62" s="4">
+      <c r="K62" s="13">
         <f t="shared" si="5"/>
         <v>88.699999999999989</v>
       </c>
@@ -4695,7 +4694,7 @@
       <c r="F63">
         <v>85</v>
       </c>
-      <c r="G63" s="9">
+      <c r="G63" s="14">
         <f t="shared" si="3"/>
         <v>61.25</v>
       </c>
@@ -4705,11 +4704,11 @@
       <c r="I63">
         <v>23</v>
       </c>
-      <c r="J63" s="13">
+      <c r="J63" s="10">
         <f t="shared" si="4"/>
         <v>65.5</v>
       </c>
-      <c r="K63" s="4">
+      <c r="K63" s="13">
         <f t="shared" si="5"/>
         <v>63.8</v>
       </c>
@@ -4733,21 +4732,21 @@
       <c r="F64">
         <v>55</v>
       </c>
-      <c r="G64" s="9">
+      <c r="G64" s="14">
         <f t="shared" si="3"/>
         <v>66.25</v>
       </c>
-      <c r="H64" s="15">
+      <c r="H64" s="7">
         <v>34</v>
       </c>
-      <c r="I64" s="15">
+      <c r="I64" s="7">
         <v>22</v>
       </c>
-      <c r="J64" s="13">
+      <c r="J64" s="10">
         <f t="shared" si="4"/>
         <v>56</v>
       </c>
-      <c r="K64" s="4">
+      <c r="K64" s="13">
         <f t="shared" si="5"/>
         <v>60.1</v>
       </c>
@@ -4771,7 +4770,7 @@
       <c r="F65">
         <v>100</v>
       </c>
-      <c r="G65" s="9">
+      <c r="G65" s="14">
         <f t="shared" si="3"/>
         <v>90</v>
       </c>
@@ -4781,11 +4780,11 @@
       <c r="I65">
         <v>34</v>
       </c>
-      <c r="J65" s="13">
+      <c r="J65" s="10">
         <f t="shared" si="4"/>
         <v>79</v>
       </c>
-      <c r="K65" s="4">
+      <c r="K65" s="13">
         <f t="shared" si="5"/>
         <v>83.4</v>
       </c>
@@ -4809,21 +4808,21 @@
       <c r="F66">
         <v>90</v>
       </c>
-      <c r="G66" s="9">
+      <c r="G66" s="14">
         <f t="shared" si="3"/>
         <v>82.5</v>
       </c>
       <c r="H66">
         <v>45</v>
       </c>
-      <c r="I66" s="15">
+      <c r="I66" s="7">
         <v>34</v>
       </c>
-      <c r="J66" s="13">
+      <c r="J66" s="10">
         <f t="shared" si="4"/>
         <v>79</v>
       </c>
-      <c r="K66" s="4">
+      <c r="K66" s="13">
         <f t="shared" si="5"/>
         <v>80.400000000000006</v>
       </c>
@@ -4847,21 +4846,21 @@
       <c r="F67">
         <v>90</v>
       </c>
-      <c r="G67" s="9">
+      <c r="G67" s="14">
         <f t="shared" ref="G67:G98" si="6">D67*0.25+E67*0.5+F67*0.25</f>
         <v>76.25</v>
       </c>
-      <c r="H67" s="15">
+      <c r="H67" s="7">
         <v>40</v>
       </c>
-      <c r="I67" s="15">
+      <c r="I67" s="7">
         <v>35</v>
       </c>
-      <c r="J67" s="13">
+      <c r="J67" s="10">
         <f t="shared" ref="J67:J98" si="7">H67+I67</f>
         <v>75</v>
       </c>
-      <c r="K67" s="4">
+      <c r="K67" s="13">
         <f t="shared" ref="K67:K98" si="8">(G67*0.4)+(J67*0.6)</f>
         <v>75.5</v>
       </c>
@@ -4882,18 +4881,18 @@
       <c r="F68">
         <v>95</v>
       </c>
-      <c r="G68" s="9">
+      <c r="G68" s="14">
         <f t="shared" si="6"/>
         <v>53.75</v>
       </c>
       <c r="H68">
         <v>0</v>
       </c>
-      <c r="J68" s="13">
+      <c r="J68" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K68" s="4">
+      <c r="K68" s="13">
         <f t="shared" si="8"/>
         <v>21.5</v>
       </c>
@@ -4917,21 +4916,21 @@
       <c r="F69">
         <v>100</v>
       </c>
-      <c r="G69" s="9">
+      <c r="G69" s="14">
         <f t="shared" si="6"/>
         <v>85</v>
       </c>
       <c r="H69">
         <v>50</v>
       </c>
-      <c r="I69" s="15">
+      <c r="I69" s="7">
         <v>44</v>
       </c>
-      <c r="J69" s="13">
+      <c r="J69" s="10">
         <f t="shared" si="7"/>
         <v>94</v>
       </c>
-      <c r="K69" s="4">
+      <c r="K69" s="13">
         <f t="shared" si="8"/>
         <v>90.4</v>
       </c>
@@ -4955,21 +4954,21 @@
       <c r="F70">
         <v>90</v>
       </c>
-      <c r="G70" s="9">
+      <c r="G70" s="14">
         <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="H70" s="15">
+      <c r="H70" s="7">
         <v>25</v>
       </c>
       <c r="I70">
         <v>37</v>
       </c>
-      <c r="J70" s="13">
+      <c r="J70" s="10">
         <f t="shared" si="7"/>
         <v>62</v>
       </c>
-      <c r="K70" s="4">
+      <c r="K70" s="13">
         <f t="shared" si="8"/>
         <v>70.199999999999989</v>
       </c>
@@ -4993,7 +4992,7 @@
       <c r="F71">
         <v>85</v>
       </c>
-      <c r="G71" s="9">
+      <c r="G71" s="14">
         <f t="shared" si="6"/>
         <v>87.5</v>
       </c>
@@ -5003,11 +5002,11 @@
       <c r="I71">
         <v>9</v>
       </c>
-      <c r="J71" s="13">
+      <c r="J71" s="10">
         <f t="shared" si="7"/>
         <v>51.5</v>
       </c>
-      <c r="K71" s="4">
+      <c r="K71" s="13">
         <f t="shared" si="8"/>
         <v>65.900000000000006</v>
       </c>
@@ -5031,21 +5030,21 @@
       <c r="F72">
         <v>95</v>
       </c>
-      <c r="G72" s="9">
+      <c r="G72" s="14">
         <f t="shared" si="6"/>
         <v>83.75</v>
       </c>
       <c r="H72">
         <v>45</v>
       </c>
-      <c r="I72" s="15">
+      <c r="I72" s="7">
         <v>33</v>
       </c>
-      <c r="J72" s="13">
+      <c r="J72" s="10">
         <f t="shared" si="7"/>
         <v>78</v>
       </c>
-      <c r="K72" s="4">
+      <c r="K72" s="13">
         <f t="shared" si="8"/>
         <v>80.3</v>
       </c>
@@ -5069,21 +5068,21 @@
       <c r="F73">
         <v>80</v>
       </c>
-      <c r="G73" s="9">
+      <c r="G73" s="14">
         <f t="shared" si="6"/>
         <v>87.5</v>
       </c>
       <c r="H73">
         <v>50</v>
       </c>
-      <c r="I73" s="15">
+      <c r="I73" s="7">
         <v>34</v>
       </c>
-      <c r="J73" s="13">
+      <c r="J73" s="10">
         <f t="shared" si="7"/>
         <v>84</v>
       </c>
-      <c r="K73" s="4">
+      <c r="K73" s="13">
         <f t="shared" si="8"/>
         <v>85.4</v>
       </c>
@@ -5107,21 +5106,21 @@
       <c r="F74">
         <v>100</v>
       </c>
-      <c r="G74" s="9">
+      <c r="G74" s="14">
         <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="H74">
         <v>45</v>
       </c>
-      <c r="I74" s="15">
+      <c r="I74" s="7">
         <v>37</v>
       </c>
-      <c r="J74" s="13">
+      <c r="J74" s="10">
         <f t="shared" si="7"/>
         <v>82</v>
       </c>
-      <c r="K74" s="4">
+      <c r="K74" s="13">
         <f t="shared" si="8"/>
         <v>85.199999999999989</v>
       </c>
@@ -5145,7 +5144,7 @@
       <c r="F75">
         <v>90</v>
       </c>
-      <c r="G75" s="9">
+      <c r="G75" s="14">
         <f t="shared" si="6"/>
         <v>80</v>
       </c>
@@ -5155,11 +5154,11 @@
       <c r="I75">
         <v>21</v>
       </c>
-      <c r="J75" s="13">
+      <c r="J75" s="10">
         <f t="shared" si="7"/>
         <v>66</v>
       </c>
-      <c r="K75" s="4">
+      <c r="K75" s="13">
         <f t="shared" si="8"/>
         <v>71.599999999999994</v>
       </c>
@@ -5174,18 +5173,18 @@
       <c r="C76" t="s">
         <v>224</v>
       </c>
-      <c r="G76" s="9">
+      <c r="G76" s="14">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H76">
         <v>0</v>
       </c>
-      <c r="J76" s="13">
+      <c r="J76" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K76" s="4">
+      <c r="K76" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -5203,21 +5202,21 @@
       <c r="E77">
         <v>60</v>
       </c>
-      <c r="G77" s="9">
+      <c r="G77" s="14">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
-      <c r="H77" s="15">
+      <c r="H77" s="7">
         <v>45</v>
       </c>
-      <c r="I77" s="15">
+      <c r="I77" s="7">
         <v>35</v>
       </c>
-      <c r="J77" s="13">
+      <c r="J77" s="10">
         <f t="shared" si="7"/>
         <v>80</v>
       </c>
-      <c r="K77" s="4">
+      <c r="K77" s="13">
         <f t="shared" si="8"/>
         <v>60</v>
       </c>
@@ -5241,21 +5240,21 @@
       <c r="F78">
         <v>100</v>
       </c>
-      <c r="G78" s="9">
+      <c r="G78" s="14">
         <f t="shared" si="6"/>
         <v>90</v>
       </c>
       <c r="H78">
         <v>45</v>
       </c>
-      <c r="I78" s="15">
+      <c r="I78" s="7">
         <v>29</v>
       </c>
-      <c r="J78" s="13">
+      <c r="J78" s="10">
         <f t="shared" si="7"/>
         <v>74</v>
       </c>
-      <c r="K78" s="4">
+      <c r="K78" s="13">
         <f t="shared" si="8"/>
         <v>80.400000000000006</v>
       </c>
@@ -5273,18 +5272,18 @@
       <c r="E79">
         <v>40</v>
       </c>
-      <c r="G79" s="9">
+      <c r="G79" s="14">
         <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="H79">
         <v>0</v>
       </c>
-      <c r="J79" s="13">
+      <c r="J79" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K79" s="4">
+      <c r="K79" s="13">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
@@ -5308,7 +5307,7 @@
       <c r="F80">
         <v>80</v>
       </c>
-      <c r="G80" s="9">
+      <c r="G80" s="14">
         <f t="shared" si="6"/>
         <v>80</v>
       </c>
@@ -5318,11 +5317,11 @@
       <c r="I80">
         <v>25</v>
       </c>
-      <c r="J80" s="13">
+      <c r="J80" s="10">
         <f t="shared" si="7"/>
         <v>65</v>
       </c>
-      <c r="K80" s="4">
+      <c r="K80" s="13">
         <f t="shared" si="8"/>
         <v>71</v>
       </c>
@@ -5346,21 +5345,21 @@
       <c r="F81">
         <v>100</v>
       </c>
-      <c r="G81" s="9">
+      <c r="G81" s="14">
         <f t="shared" si="6"/>
         <v>80</v>
       </c>
       <c r="H81">
         <v>45</v>
       </c>
-      <c r="I81" s="15">
+      <c r="I81" s="7">
         <v>44</v>
       </c>
-      <c r="J81" s="13">
+      <c r="J81" s="10">
         <f t="shared" si="7"/>
         <v>89</v>
       </c>
-      <c r="K81" s="4">
+      <c r="K81" s="13">
         <f t="shared" si="8"/>
         <v>85.4</v>
       </c>
@@ -5384,21 +5383,21 @@
       <c r="F82">
         <v>95</v>
       </c>
-      <c r="G82" s="9">
+      <c r="G82" s="14">
         <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="H82" s="15">
+      <c r="H82" s="7">
         <v>48</v>
       </c>
       <c r="I82">
         <v>47</v>
       </c>
-      <c r="J82" s="13">
+      <c r="J82" s="10">
         <f t="shared" si="7"/>
         <v>95</v>
       </c>
-      <c r="K82" s="4">
+      <c r="K82" s="13">
         <f t="shared" si="8"/>
         <v>90</v>
       </c>
@@ -5413,18 +5412,18 @@
       <c r="C83" t="s">
         <v>245</v>
       </c>
-      <c r="G83" s="9">
+      <c r="G83" s="14">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H83">
         <v>0</v>
       </c>
-      <c r="J83" s="13">
+      <c r="J83" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K83" s="4">
+      <c r="K83" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -5448,21 +5447,21 @@
       <c r="F84">
         <v>70</v>
       </c>
-      <c r="G84" s="9">
+      <c r="G84" s="14">
         <f t="shared" si="6"/>
         <v>82.5</v>
       </c>
-      <c r="H84" s="15">
+      <c r="H84" s="7">
         <v>46</v>
       </c>
       <c r="I84">
         <v>33</v>
       </c>
-      <c r="J84" s="13">
+      <c r="J84" s="10">
         <f t="shared" si="7"/>
         <v>79</v>
       </c>
-      <c r="K84" s="4">
+      <c r="K84" s="13">
         <f t="shared" si="8"/>
         <v>80.400000000000006</v>
       </c>
@@ -5486,7 +5485,7 @@
       <c r="F85">
         <v>85</v>
       </c>
-      <c r="G85" s="9">
+      <c r="G85" s="14">
         <f t="shared" si="6"/>
         <v>76.25</v>
       </c>
@@ -5496,11 +5495,11 @@
       <c r="I85">
         <v>24</v>
       </c>
-      <c r="J85" s="13">
+      <c r="J85" s="10">
         <f t="shared" si="7"/>
         <v>66.5</v>
       </c>
-      <c r="K85" s="4">
+      <c r="K85" s="13">
         <f t="shared" si="8"/>
         <v>70.400000000000006</v>
       </c>
@@ -5524,7 +5523,7 @@
       <c r="F86">
         <v>45</v>
       </c>
-      <c r="G86" s="9">
+      <c r="G86" s="14">
         <f t="shared" si="6"/>
         <v>38.75</v>
       </c>
@@ -5534,11 +5533,11 @@
       <c r="I86">
         <v>20</v>
       </c>
-      <c r="J86" s="13">
+      <c r="J86" s="10">
         <f t="shared" si="7"/>
         <v>30</v>
       </c>
-      <c r="K86" s="4">
+      <c r="K86" s="13">
         <f t="shared" si="8"/>
         <v>33.5</v>
       </c>
@@ -5556,7 +5555,7 @@
       <c r="E87">
         <v>60</v>
       </c>
-      <c r="G87" s="9">
+      <c r="G87" s="14">
         <f t="shared" si="6"/>
         <v>30</v>
       </c>
@@ -5566,11 +5565,11 @@
       <c r="I87">
         <v>42</v>
       </c>
-      <c r="J87" s="13">
+      <c r="J87" s="10">
         <f t="shared" si="7"/>
         <v>82</v>
       </c>
-      <c r="K87" s="4">
+      <c r="K87" s="13">
         <f t="shared" si="8"/>
         <v>61.199999999999996</v>
       </c>
@@ -5594,7 +5593,7 @@
       <c r="F88">
         <v>95</v>
       </c>
-      <c r="G88" s="9">
+      <c r="G88" s="14">
         <f t="shared" si="6"/>
         <v>76.25</v>
       </c>
@@ -5604,11 +5603,11 @@
       <c r="I88">
         <v>12</v>
       </c>
-      <c r="J88" s="13">
+      <c r="J88" s="10">
         <f t="shared" si="7"/>
         <v>50</v>
       </c>
-      <c r="K88" s="4">
+      <c r="K88" s="13">
         <f t="shared" si="8"/>
         <v>60.5</v>
       </c>
@@ -5632,7 +5631,7 @@
       <c r="F89">
         <v>75</v>
       </c>
-      <c r="G89" s="9">
+      <c r="G89" s="14">
         <f t="shared" si="6"/>
         <v>63.75</v>
       </c>
@@ -5642,11 +5641,11 @@
       <c r="I89">
         <v>3</v>
       </c>
-      <c r="J89" s="13">
+      <c r="J89" s="10">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="K89" s="4">
+      <c r="K89" s="13">
         <f t="shared" si="8"/>
         <v>27.3</v>
       </c>
@@ -5670,21 +5669,21 @@
       <c r="F90">
         <v>85</v>
       </c>
-      <c r="G90" s="9">
+      <c r="G90" s="14">
         <f t="shared" si="6"/>
         <v>62.5</v>
       </c>
       <c r="H90">
         <v>40</v>
       </c>
-      <c r="I90" s="15">
+      <c r="I90" s="7">
         <v>28</v>
       </c>
-      <c r="J90" s="13">
+      <c r="J90" s="10">
         <f t="shared" si="7"/>
         <v>68</v>
       </c>
-      <c r="K90" s="4">
+      <c r="K90" s="13">
         <f t="shared" si="8"/>
         <v>65.8</v>
       </c>
@@ -5702,18 +5701,18 @@
       <c r="E91">
         <v>35</v>
       </c>
-      <c r="G91" s="9">
+      <c r="G91" s="14">
         <f t="shared" si="6"/>
         <v>17.5</v>
       </c>
       <c r="H91">
         <v>0</v>
       </c>
-      <c r="J91" s="13">
+      <c r="J91" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K91" s="4">
+      <c r="K91" s="13">
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
@@ -5737,7 +5736,7 @@
       <c r="F92">
         <v>90</v>
       </c>
-      <c r="G92" s="9">
+      <c r="G92" s="14">
         <f t="shared" si="6"/>
         <v>80</v>
       </c>
@@ -5747,11 +5746,11 @@
       <c r="I92">
         <v>30</v>
       </c>
-      <c r="J92" s="13">
+      <c r="J92" s="10">
         <f t="shared" si="7"/>
         <v>72.5</v>
       </c>
-      <c r="K92" s="4">
+      <c r="K92" s="13">
         <f t="shared" si="8"/>
         <v>75.5</v>
       </c>
@@ -5775,7 +5774,7 @@
       <c r="F93">
         <v>90</v>
       </c>
-      <c r="G93" s="9">
+      <c r="G93" s="14">
         <f t="shared" si="6"/>
         <v>92.5</v>
       </c>
@@ -5785,11 +5784,11 @@
       <c r="I93">
         <v>24</v>
       </c>
-      <c r="J93" s="13">
+      <c r="J93" s="10">
         <f t="shared" si="7"/>
         <v>74</v>
       </c>
-      <c r="K93" s="4">
+      <c r="K93" s="13">
         <f t="shared" si="8"/>
         <v>81.400000000000006</v>
       </c>
@@ -5813,21 +5812,21 @@
       <c r="F94">
         <v>100</v>
       </c>
-      <c r="G94" s="9">
+      <c r="G94" s="14">
         <f t="shared" si="6"/>
         <v>87.5</v>
       </c>
       <c r="H94">
         <v>50</v>
       </c>
-      <c r="I94" s="15">
+      <c r="I94" s="7">
         <v>42</v>
       </c>
-      <c r="J94" s="13">
+      <c r="J94" s="10">
         <f t="shared" si="7"/>
         <v>92</v>
       </c>
-      <c r="K94" s="4">
+      <c r="K94" s="13">
         <f t="shared" si="8"/>
         <v>90.199999999999989</v>
       </c>
@@ -5845,18 +5844,18 @@
       <c r="E95">
         <v>50</v>
       </c>
-      <c r="G95" s="9">
+      <c r="G95" s="14">
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="H95">
         <v>0</v>
       </c>
-      <c r="J95" s="13">
+      <c r="J95" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K95" s="4">
+      <c r="K95" s="13">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
@@ -5880,7 +5879,7 @@
       <c r="F96">
         <v>100</v>
       </c>
-      <c r="G96" s="9">
+      <c r="G96" s="14">
         <f t="shared" si="6"/>
         <v>87.5</v>
       </c>
@@ -5890,11 +5889,11 @@
       <c r="I96">
         <v>48</v>
       </c>
-      <c r="J96" s="13">
+      <c r="J96" s="10">
         <f t="shared" si="7"/>
         <v>98</v>
       </c>
-      <c r="K96" s="4">
+      <c r="K96" s="13">
         <f t="shared" si="8"/>
         <v>93.8</v>
       </c>
@@ -5918,7 +5917,7 @@
       <c r="F97">
         <v>85</v>
       </c>
-      <c r="G97" s="9">
+      <c r="G97" s="14">
         <f t="shared" si="6"/>
         <v>68.75</v>
       </c>
@@ -5928,11 +5927,11 @@
       <c r="I97">
         <v>34</v>
       </c>
-      <c r="J97" s="13">
+      <c r="J97" s="10">
         <f t="shared" si="7"/>
         <v>80</v>
       </c>
-      <c r="K97" s="4">
+      <c r="K97" s="13">
         <f t="shared" si="8"/>
         <v>75.5</v>
       </c>
@@ -5947,18 +5946,18 @@
       <c r="C98" t="s">
         <v>290</v>
       </c>
-      <c r="G98" s="9">
+      <c r="G98" s="14">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H98">
         <v>0</v>
       </c>
-      <c r="J98" s="13">
+      <c r="J98" s="10">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K98" s="4">
+      <c r="K98" s="13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -5982,7 +5981,7 @@
       <c r="F99">
         <v>55</v>
       </c>
-      <c r="G99" s="9">
+      <c r="G99" s="14">
         <f t="shared" ref="G99:G117" si="9">D99*0.25+E99*0.5+F99*0.25</f>
         <v>75</v>
       </c>
@@ -5992,11 +5991,11 @@
       <c r="I99">
         <v>16</v>
       </c>
-      <c r="J99" s="13">
+      <c r="J99" s="10">
         <f t="shared" ref="J99:J117" si="10">H99+I99</f>
         <v>58.5</v>
       </c>
-      <c r="K99" s="4">
+      <c r="K99" s="13">
         <f t="shared" ref="K99:K117" si="11">(G99*0.4)+(J99*0.6)</f>
         <v>65.099999999999994</v>
       </c>
@@ -6020,18 +6019,18 @@
       <c r="F100">
         <v>55</v>
       </c>
-      <c r="G100" s="9">
+      <c r="G100" s="14">
         <f t="shared" si="9"/>
         <v>63.75</v>
       </c>
       <c r="H100">
         <v>0</v>
       </c>
-      <c r="J100" s="13">
+      <c r="J100" s="10">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="K100" s="4">
+      <c r="K100" s="13">
         <f t="shared" si="11"/>
         <v>25.5</v>
       </c>
@@ -6049,18 +6048,18 @@
       <c r="E101">
         <v>100</v>
       </c>
-      <c r="G101" s="9">
+      <c r="G101" s="14">
         <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="H101">
         <v>40</v>
       </c>
-      <c r="J101" s="13">
+      <c r="J101" s="10">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="K101" s="4">
+      <c r="K101" s="13">
         <f t="shared" si="11"/>
         <v>44</v>
       </c>
@@ -6084,21 +6083,21 @@
       <c r="F102">
         <v>85</v>
       </c>
-      <c r="G102" s="9">
+      <c r="G102" s="14">
         <f t="shared" si="9"/>
         <v>71.25</v>
       </c>
-      <c r="H102" s="15">
+      <c r="H102" s="7">
         <v>33</v>
       </c>
-      <c r="I102" s="15">
+      <c r="I102" s="7">
         <v>20</v>
       </c>
-      <c r="J102" s="13">
+      <c r="J102" s="10">
         <f t="shared" si="10"/>
         <v>53</v>
       </c>
-      <c r="K102" s="4">
+      <c r="K102" s="13">
         <f t="shared" si="11"/>
         <v>60.3</v>
       </c>
@@ -6122,7 +6121,7 @@
       <c r="F103">
         <v>85</v>
       </c>
-      <c r="G103" s="9">
+      <c r="G103" s="14">
         <f t="shared" si="9"/>
         <v>83.75</v>
       </c>
@@ -6132,11 +6131,11 @@
       <c r="I103">
         <v>37</v>
       </c>
-      <c r="J103" s="13">
+      <c r="J103" s="10">
         <f t="shared" si="10"/>
         <v>79.5</v>
       </c>
-      <c r="K103" s="4">
+      <c r="K103" s="13">
         <f t="shared" si="11"/>
         <v>81.199999999999989</v>
       </c>
@@ -6157,21 +6156,21 @@
       <c r="F104">
         <v>60</v>
       </c>
-      <c r="G104" s="9">
+      <c r="G104" s="14">
         <f t="shared" si="9"/>
         <v>47.5</v>
       </c>
-      <c r="H104" s="15">
+      <c r="H104" s="7">
         <v>43</v>
       </c>
-      <c r="I104" s="15">
+      <c r="I104" s="7">
         <v>26</v>
       </c>
-      <c r="J104" s="13">
+      <c r="J104" s="10">
         <f t="shared" si="10"/>
         <v>69</v>
       </c>
-      <c r="K104" s="4">
+      <c r="K104" s="13">
         <f t="shared" si="11"/>
         <v>60.4</v>
       </c>
@@ -6195,21 +6194,21 @@
       <c r="F105">
         <v>85</v>
       </c>
-      <c r="G105" s="9">
+      <c r="G105" s="14">
         <f t="shared" si="9"/>
         <v>68.75</v>
       </c>
-      <c r="H105" s="15">
+      <c r="H105" s="7">
         <v>42</v>
       </c>
-      <c r="I105" s="15">
+      <c r="I105" s="7">
         <v>38</v>
       </c>
-      <c r="J105" s="13">
+      <c r="J105" s="10">
         <f t="shared" si="10"/>
         <v>80</v>
       </c>
-      <c r="K105" s="4">
+      <c r="K105" s="13">
         <f t="shared" si="11"/>
         <v>75.5</v>
       </c>
@@ -6233,7 +6232,7 @@
       <c r="F106">
         <v>75</v>
       </c>
-      <c r="G106" s="9">
+      <c r="G106" s="14">
         <f t="shared" si="9"/>
         <v>81.25</v>
       </c>
@@ -6243,11 +6242,11 @@
       <c r="I106">
         <v>28</v>
       </c>
-      <c r="J106" s="13">
+      <c r="J106" s="10">
         <f t="shared" si="10"/>
         <v>58</v>
       </c>
-      <c r="K106" s="4">
+      <c r="K106" s="13">
         <f t="shared" si="11"/>
         <v>67.3</v>
       </c>
@@ -6271,21 +6270,21 @@
       <c r="F107">
         <v>100</v>
       </c>
-      <c r="G107" s="9">
+      <c r="G107" s="14">
         <f t="shared" si="9"/>
         <v>75</v>
       </c>
-      <c r="H107" s="15">
+      <c r="H107" s="7">
         <v>48</v>
       </c>
       <c r="I107">
         <v>36</v>
       </c>
-      <c r="J107" s="13">
+      <c r="J107" s="10">
         <f t="shared" si="10"/>
         <v>84</v>
       </c>
-      <c r="K107" s="4">
+      <c r="K107" s="13">
         <f t="shared" si="11"/>
         <v>80.400000000000006</v>
       </c>
@@ -6309,21 +6308,21 @@
       <c r="F108">
         <v>95</v>
       </c>
-      <c r="G108" s="9">
+      <c r="G108" s="14">
         <f t="shared" si="9"/>
         <v>73.75</v>
       </c>
-      <c r="H108" s="15">
+      <c r="H108" s="7">
         <v>44</v>
       </c>
       <c r="I108">
         <v>32</v>
       </c>
-      <c r="J108" s="13">
+      <c r="J108" s="10">
         <f t="shared" si="10"/>
         <v>76</v>
       </c>
-      <c r="K108" s="4">
+      <c r="K108" s="13">
         <f t="shared" si="11"/>
         <v>75.099999999999994</v>
       </c>
@@ -6347,7 +6346,7 @@
       <c r="F109">
         <v>85</v>
       </c>
-      <c r="G109" s="9">
+      <c r="G109" s="14">
         <f t="shared" si="9"/>
         <v>81.25</v>
       </c>
@@ -6357,11 +6356,11 @@
       <c r="I109">
         <v>26</v>
       </c>
-      <c r="J109" s="13">
+      <c r="J109" s="10">
         <f t="shared" si="10"/>
         <v>63.5</v>
       </c>
-      <c r="K109" s="4">
+      <c r="K109" s="13">
         <f t="shared" si="11"/>
         <v>70.599999999999994</v>
       </c>
@@ -6382,21 +6381,21 @@
       <c r="F110">
         <v>100</v>
       </c>
-      <c r="G110" s="9">
+      <c r="G110" s="14">
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
-      <c r="H110" s="15">
+      <c r="H110" s="7">
         <v>30</v>
       </c>
-      <c r="I110" s="15">
+      <c r="I110" s="7">
         <v>34</v>
       </c>
-      <c r="J110" s="13">
+      <c r="J110" s="10">
         <f t="shared" si="10"/>
         <v>64</v>
       </c>
-      <c r="K110" s="4">
+      <c r="K110" s="13">
         <f t="shared" si="11"/>
         <v>60.4</v>
       </c>
@@ -6420,21 +6419,21 @@
       <c r="F111">
         <v>85</v>
       </c>
-      <c r="G111" s="9">
+      <c r="G111" s="14">
         <f t="shared" si="9"/>
         <v>78.75</v>
       </c>
       <c r="H111">
         <v>50</v>
       </c>
-      <c r="I111" s="15">
+      <c r="I111" s="7">
         <v>48</v>
       </c>
-      <c r="J111" s="13">
+      <c r="J111" s="10">
         <f t="shared" si="10"/>
         <v>98</v>
       </c>
-      <c r="K111" s="4">
+      <c r="K111" s="13">
         <f t="shared" si="11"/>
         <v>90.3</v>
       </c>
@@ -6458,7 +6457,7 @@
       <c r="F112">
         <v>100</v>
       </c>
-      <c r="G112" s="9">
+      <c r="G112" s="14">
         <f t="shared" si="9"/>
         <v>90</v>
       </c>
@@ -6468,11 +6467,11 @@
       <c r="I112">
         <v>45</v>
       </c>
-      <c r="J112" s="13">
+      <c r="J112" s="10">
         <f t="shared" si="10"/>
         <v>95</v>
       </c>
-      <c r="K112" s="4">
+      <c r="K112" s="13">
         <f t="shared" si="11"/>
         <v>93</v>
       </c>
@@ -6490,7 +6489,7 @@
       <c r="E113">
         <v>45</v>
       </c>
-      <c r="G113" s="9">
+      <c r="G113" s="14">
         <f t="shared" si="9"/>
         <v>22.5</v>
       </c>
@@ -6500,11 +6499,11 @@
       <c r="I113">
         <v>2</v>
       </c>
-      <c r="J113" s="13">
+      <c r="J113" s="10">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="K113" s="4">
+      <c r="K113" s="13">
         <f t="shared" si="11"/>
         <v>10.199999999999999</v>
       </c>
@@ -6525,7 +6524,7 @@
       <c r="F114">
         <v>80</v>
       </c>
-      <c r="G114" s="9">
+      <c r="G114" s="14">
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
@@ -6535,11 +6534,11 @@
       <c r="I114">
         <v>14</v>
       </c>
-      <c r="J114" s="13">
+      <c r="J114" s="10">
         <f t="shared" si="10"/>
         <v>64</v>
       </c>
-      <c r="K114" s="4">
+      <c r="K114" s="13">
         <f t="shared" si="11"/>
         <v>60.4</v>
       </c>
@@ -6557,7 +6556,7 @@
       <c r="E115">
         <v>90</v>
       </c>
-      <c r="G115" s="9">
+      <c r="G115" s="14">
         <f t="shared" si="9"/>
         <v>45</v>
       </c>
@@ -6567,11 +6566,11 @@
       <c r="I115">
         <v>14</v>
       </c>
-      <c r="J115" s="13">
+      <c r="J115" s="10">
         <f t="shared" si="10"/>
         <v>14</v>
       </c>
-      <c r="K115" s="4">
+      <c r="K115" s="13">
         <f t="shared" si="11"/>
         <v>26.4</v>
       </c>
@@ -6595,21 +6594,21 @@
       <c r="F116">
         <v>90</v>
       </c>
-      <c r="G116" s="9">
+      <c r="G116" s="14">
         <f t="shared" si="9"/>
         <v>76.25</v>
       </c>
-      <c r="H116" s="15">
+      <c r="H116" s="7">
         <v>50</v>
       </c>
       <c r="I116">
         <v>50</v>
       </c>
-      <c r="J116" s="13">
+      <c r="J116" s="10">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="K116" s="4">
+      <c r="K116" s="13">
         <f t="shared" si="11"/>
         <v>90.5</v>
       </c>
@@ -6633,7 +6632,7 @@
       <c r="F117">
         <v>90</v>
       </c>
-      <c r="G117" s="9">
+      <c r="G117" s="14">
         <f t="shared" si="9"/>
         <v>95</v>
       </c>
@@ -6643,11 +6642,11 @@
       <c r="I117">
         <v>50</v>
       </c>
-      <c r="J117" s="13">
+      <c r="J117" s="10">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
-      <c r="K117" s="4">
+      <c r="K117" s="13">
         <f t="shared" si="11"/>
         <v>98</v>
       </c>
@@ -6666,585 +6665,585 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D1D592F-937B-D149-BB0B-8ED9164C109C}">
   <dimension ref="A1:A115"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1">
-        <v>98</v>
+        <v>61.7</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>95</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>94.3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>94.199999999999989</v>
+        <v>75.400000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>93.8</v>
+        <v>94.199999999999989</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>93.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>93</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>89.5</v>
+        <v>70.3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>89.4</v>
+        <v>77.900000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>89.199999999999989</v>
+        <v>90.8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>89.199999999999989</v>
+        <v>67.3</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>88.699999999999989</v>
+        <v>83.8</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>88.5</v>
+        <v>93.3</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>88.5</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>88.4</v>
+        <v>90.1</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>88.4</v>
+        <v>94.3</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>88.3</v>
+        <v>90.1</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>88.199999999999989</v>
+        <v>72.199999999999989</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>87.8</v>
+        <v>70.699999999999989</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>87.5</v>
+        <v>60.1</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>84.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>84.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>83.8</v>
+        <v>60.199999999999996</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>83.4</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>83.4</v>
+        <v>75.900000000000006</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>83.3</v>
+        <v>85.5</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>83</v>
+        <v>70.699999999999989</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>82.4</v>
+        <v>71.900000000000006</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>81.400000000000006</v>
+        <v>81.099999999999994</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>81.199999999999989</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>81.099999999999994</v>
+        <v>61.5</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>80.400000000000006</v>
+        <v>80.099999999999994</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>79.8</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>79.8</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>78.900000000000006</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>78.599999999999994</v>
+        <v>70.5</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>78.599999999999994</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>78.5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>77.900000000000006</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>77.900000000000006</v>
+        <v>65.400000000000006</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>75.699999999999989</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>75.5</v>
+        <v>75.699999999999989</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>74.400000000000006</v>
+        <v>65.400000000000006</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>74.099999999999994</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>73.8</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>73.599999999999994</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>73.400000000000006</v>
+        <v>85.3</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>73</v>
+        <v>70.900000000000006</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>73</v>
+        <v>66.3</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>72.699999999999989</v>
+        <v>66.900000000000006</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>72.5</v>
+        <v>62.199999999999996</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>72.199999999999989</v>
+        <v>60.3</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>72.199999999999989</v>
+        <v>90.199999999999989</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>71.900000000000006</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>71.599999999999994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>71</v>
+        <v>78.5</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>70.900000000000006</v>
+        <v>66</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>70.699999999999989</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>70.699999999999989</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>70.599999999999994</v>
+        <v>88.699999999999989</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>70.400000000000006</v>
+        <v>63.8</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>70</v>
+        <v>60.1</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>69.900000000000006</v>
+        <v>83.4</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>68.699999999999989</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>68.400000000000006</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>67.3</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>67.3</v>
+        <v>90.4</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>67.3</v>
+        <v>70.199999999999989</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>66.900000000000006</v>
+        <v>65.900000000000006</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>66.3</v>
+        <v>80.3</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>66</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>65.900000000000006</v>
+        <v>85.199999999999989</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>65.099999999999994</v>
+        <v>71.599999999999994</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>64.599999999999994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>64.2</v>
+        <v>60</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>63.8</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>63</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>62.199999999999996</v>
+        <v>71</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>61.7</v>
+        <v>85.4</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>61.5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>61.199999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>61</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>60.5</v>
+        <v>70.400000000000006</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>60</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>55.9</v>
+        <v>61.199999999999996</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>53.6</v>
+        <v>60.5</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>53.5</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>53.199999999999996</v>
+        <v>65.8</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>52.9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>50.5</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>49.2</v>
+        <v>81.400000000000006</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>48.7</v>
+        <v>90.199999999999989</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>47.7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>45.9</v>
+        <v>93.8</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>44</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>38</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>35.9</v>
+        <v>65.099999999999994</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>33.5</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>27.3</v>
+        <v>60.3</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>26.4</v>
+        <v>81.199999999999989</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>25.5</v>
+        <v>60.4</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>21.5</v>
+        <v>75.5</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>15</v>
+        <v>67.3</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>10.199999999999999</v>
+        <v>80.400000000000006</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>10</v>
+        <v>75.099999999999994</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>8</v>
+        <v>70.599999999999994</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>7</v>
+        <v>60.4</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>0</v>
+        <v>90.3</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>0</v>
+        <v>93</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>0</v>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>0</v>
+        <v>60.4</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>0</v>
+        <v>26.4</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>0</v>
+        <v>90.5</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>0</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -7257,955 +7256,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CAB4FD3-C627-EE4A-87DC-E610ACDA7C75}">
-  <dimension ref="A1:B116"/>
-  <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>100</v>
-      </c>
-      <c r="B1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>95</v>
-      </c>
-      <c r="B2">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>98</v>
-      </c>
-      <c r="B3">
-        <v>94.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>94.5</v>
-      </c>
-      <c r="B4">
-        <v>94.199999999999989</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>98</v>
-      </c>
-      <c r="B5">
-        <v>93.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>98</v>
-      </c>
-      <c r="B6">
-        <v>93.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>95</v>
-      </c>
-      <c r="B7">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>88</v>
-      </c>
-      <c r="B8">
-        <v>90.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>100</v>
-      </c>
-      <c r="B9">
-        <v>90.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>94</v>
-      </c>
-      <c r="B10">
-        <v>90.4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>94</v>
-      </c>
-      <c r="B11">
-        <v>90.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>98</v>
-      </c>
-      <c r="B12">
-        <v>90.3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>97</v>
-      </c>
-      <c r="B13">
-        <v>90.199999999999989</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>92</v>
-      </c>
-      <c r="B14">
-        <v>90.199999999999989</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>96</v>
-      </c>
-      <c r="B15">
-        <v>90.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>91</v>
-      </c>
-      <c r="B16">
-        <v>90.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>90</v>
-      </c>
-      <c r="B17">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>90</v>
-      </c>
-      <c r="B18">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>95</v>
-      </c>
-      <c r="B19">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>92</v>
-      </c>
-      <c r="B20">
-        <v>88.699999999999989</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>85</v>
-      </c>
-      <c r="B21">
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>84</v>
-      </c>
-      <c r="B22">
-        <v>85.4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>84</v>
-      </c>
-      <c r="B23">
-        <v>85.4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>89</v>
-      </c>
-      <c r="B24">
-        <v>85.4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>88</v>
-      </c>
-      <c r="B25">
-        <v>85.3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>82</v>
-      </c>
-      <c r="B26">
-        <v>85.199999999999989</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>93</v>
-      </c>
-      <c r="B27">
-        <v>83.8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>79</v>
-      </c>
-      <c r="B28">
-        <v>83.4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>74</v>
-      </c>
-      <c r="B29">
-        <v>81.400000000000006</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>79.5</v>
-      </c>
-      <c r="B30">
-        <v>81.199999999999989</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>81</v>
-      </c>
-      <c r="B31">
-        <v>81.099999999999994</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>74</v>
-      </c>
-      <c r="B32">
-        <v>80.400000000000006</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>79</v>
-      </c>
-      <c r="B33">
-        <v>80.400000000000006</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>74</v>
-      </c>
-      <c r="B34">
-        <v>80.400000000000006</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>79</v>
-      </c>
-      <c r="B35">
-        <v>80.400000000000006</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>84</v>
-      </c>
-      <c r="B36">
-        <v>80.400000000000006</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>78</v>
-      </c>
-      <c r="B37">
-        <v>80.3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>76</v>
-      </c>
-      <c r="B38">
-        <v>80.099999999999994</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>70</v>
-      </c>
-      <c r="B39">
-        <v>78.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>69</v>
-      </c>
-      <c r="B40">
-        <v>77.900000000000006</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>74</v>
-      </c>
-      <c r="B41">
-        <v>75.900000000000006</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>67</v>
-      </c>
-      <c r="B42">
-        <v>75.699999999999989</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>75</v>
-      </c>
-      <c r="B43">
-        <v>75.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>72.5</v>
-      </c>
-      <c r="B44">
-        <v>75.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>80</v>
-      </c>
-      <c r="B45">
-        <v>75.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>80</v>
-      </c>
-      <c r="B46">
-        <v>75.5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>74</v>
-      </c>
-      <c r="B47">
-        <v>75.400000000000006</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>76</v>
-      </c>
-      <c r="B48">
-        <v>75.099999999999994</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>72.5</v>
-      </c>
-      <c r="B49">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>75</v>
-      </c>
-      <c r="B50">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>65</v>
-      </c>
-      <c r="B51">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>67.5</v>
-      </c>
-      <c r="B52">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>72</v>
-      </c>
-      <c r="B53">
-        <v>72.199999999999989</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>69</v>
-      </c>
-      <c r="B54">
-        <v>71.900000000000006</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>66</v>
-      </c>
-      <c r="B55">
-        <v>71.599999999999994</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>65</v>
-      </c>
-      <c r="B56">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>64</v>
-      </c>
-      <c r="B57">
-        <v>70.900000000000006</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>72</v>
-      </c>
-      <c r="B58">
-        <v>70.699999999999989</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>67</v>
-      </c>
-      <c r="B59">
-        <v>70.699999999999989</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>63.5</v>
-      </c>
-      <c r="B60">
-        <v>70.599999999999994</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>67.5</v>
-      </c>
-      <c r="B61">
-        <v>70.5</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>66.5</v>
-      </c>
-      <c r="B62">
-        <v>70.400000000000006</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>70.5</v>
-      </c>
-      <c r="B63">
-        <v>70.3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>62</v>
-      </c>
-      <c r="B64">
-        <v>70.199999999999989</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>67.5</v>
-      </c>
-      <c r="B65">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>60.5</v>
-      </c>
-      <c r="B66">
-        <v>67.3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>58</v>
-      </c>
-      <c r="B67">
-        <v>67.3</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>71.5</v>
-      </c>
-      <c r="B68">
-        <v>66.900000000000006</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>68</v>
-      </c>
-      <c r="B69">
-        <v>66.3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>62.5</v>
-      </c>
-      <c r="B70">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>51.5</v>
-      </c>
-      <c r="B71">
-        <v>65.900000000000006</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>68</v>
-      </c>
-      <c r="B72">
-        <v>65.8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>84</v>
-      </c>
-      <c r="B73">
-        <v>65.400000000000006</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>51.5</v>
-      </c>
-      <c r="B74">
-        <v>65.400000000000006</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>58.5</v>
-      </c>
-      <c r="B75">
-        <v>65.099999999999994</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>65.5</v>
-      </c>
-      <c r="B76">
-        <v>63.8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>57</v>
-      </c>
-      <c r="B77">
-        <v>62.199999999999996</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>52</v>
-      </c>
-      <c r="B78">
-        <v>61.7</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B79" t="e">
-        <f>SUM(#REF!)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>55</v>
-      </c>
-      <c r="B80">
-        <v>61.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>82</v>
-      </c>
-      <c r="B81">
-        <v>61.199999999999996</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82">
-        <v>70</v>
-      </c>
-      <c r="B82">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>50</v>
-      </c>
-      <c r="B83">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>65</v>
-      </c>
-      <c r="B84">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>50</v>
-      </c>
-      <c r="B85">
-        <v>60.5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>69</v>
-      </c>
-      <c r="B86">
-        <v>60.4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>64</v>
-      </c>
-      <c r="B87">
-        <v>60.4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>64</v>
-      </c>
-      <c r="B88">
-        <v>60.4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>68</v>
-      </c>
-      <c r="B89">
-        <v>60.3</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>53</v>
-      </c>
-      <c r="B90">
-        <v>60.3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>56</v>
-      </c>
-      <c r="B91">
-        <v>60.1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>56</v>
-      </c>
-      <c r="B92">
-        <v>60.1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>50</v>
-      </c>
-      <c r="B93">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>70</v>
-      </c>
-      <c r="B94">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>80</v>
-      </c>
-      <c r="B95">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>40</v>
-      </c>
-      <c r="B96">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>25</v>
-      </c>
-      <c r="B97">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>36.5</v>
-      </c>
-      <c r="B98">
-        <v>35.9</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>30</v>
-      </c>
-      <c r="B99">
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>5</v>
-      </c>
-      <c r="B100">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>3</v>
-      </c>
-      <c r="B101">
-        <v>27.3</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A102">
-        <v>14</v>
-      </c>
-      <c r="B102">
-        <v>26.4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A103">
-        <v>0</v>
-      </c>
-      <c r="B103">
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A104">
-        <v>0</v>
-      </c>
-      <c r="B104">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105">
-        <v>0</v>
-      </c>
-      <c r="B105">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106">
-        <v>2</v>
-      </c>
-      <c r="B106">
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107">
-        <v>0</v>
-      </c>
-      <c r="B107">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108">
-        <v>0</v>
-      </c>
-      <c r="B108">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109">
-        <v>0</v>
-      </c>
-      <c r="B109">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110">
-        <v>0</v>
-      </c>
-      <c r="B110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A111">
-        <v>0</v>
-      </c>
-      <c r="B111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112">
-        <v>0</v>
-      </c>
-      <c r="B112">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113">
-        <v>0</v>
-      </c>
-      <c r="B113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114">
-        <v>0</v>
-      </c>
-      <c r="B114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115">
-        <v>0</v>
-      </c>
-      <c r="B115">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116">
-        <v>0</v>
-      </c>
-      <c r="B116">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B138">
-    <sortCondition descending="1" ref="B23:B138"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3DB2D0D-2955-BA4F-A9C8-09E70872ED6D}">
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8612,7 +7667,7 @@
       <c r="B40" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="5" t="s">
         <v>373</v>
       </c>
       <c r="E40">
@@ -8623,7 +7678,7 @@
       <c r="A41" t="s">
         <v>282</v>
       </c>
-      <c r="B41" s="5"/>
+      <c r="B41" s="3"/>
       <c r="E41">
         <v>100</v>
       </c>
@@ -8635,7 +7690,7 @@
       <c r="A42" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="4" t="s">
         <v>270</v>
       </c>
       <c r="E42">

</xml_diff>